<commit_message>
Review versions of PS, DCEG, and checks
</commit_message>
<xml_diff>
--- a/S158_131/1.0.0/S-158_131_1_0_0_20251226.xlsx
+++ b/S158_131/1.0.0/S-158_131_1_0_0_20251226.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\git\S-131-Product-Specification-Development\S158_131\1.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15A1EB2-3E34-4CEE-95F3-3D8F303CA714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E7F1C9-65D1-4FBA-8B9C-184FE01EA09B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" tabRatio="647" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DeletedS131Checks!$A$1:$K$31</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">S131Checks!$K$1:$K$96</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">S131Checks!$K$1:$K$95</definedName>
     <definedName name="S101_Disposition">[1]Lists!$A$1:$A$3</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1" iterateCount="1000" concurrentCalc="0"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="472">
   <si>
     <t>Document Number</t>
   </si>
@@ -1769,9 +1769,6 @@
     <t>11.5.2</t>
   </si>
   <si>
-    <t>Nullity check</t>
-  </si>
-  <si>
     <t>6.14.3</t>
   </si>
   <si>
@@ -1784,9 +1781,6 @@
     <t>Redundancy check?</t>
   </si>
   <si>
-    <t>4.3.5</t>
-  </si>
-  <si>
     <t xml:space="preserve"> An update dataset changes the limit of a DataCoverage feature for the base dataset.</t>
   </si>
   <si>
@@ -1845,6 +1839,21 @@
   </si>
   <si>
     <t>Evaluate necessity for repetition and consider deletion of repeated instance</t>
+  </si>
+  <si>
+    <t>[7.3]; [4.3.5]</t>
+  </si>
+  <si>
+    <t>12.5.2</t>
+  </si>
+  <si>
+    <t>11.7.2</t>
+  </si>
+  <si>
+    <t>11.6.1</t>
+  </si>
+  <si>
+    <t>2.4.10.3</t>
   </si>
 </sst>
 </file>
@@ -2329,7 +2338,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2567,6 +2576,96 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2579,101 +2678,8 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2988,14 +2994,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="33.6" customHeight="1">
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="123" t="s">
         <v>384</v>
       </c>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="95"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="125"/>
       <c r="H2" s="33"/>
     </row>
     <row r="3" spans="2:8" s="9" customFormat="1" ht="20.45" customHeight="1">
@@ -3121,7 +3127,7 @@
       <c r="G12" s="34"/>
     </row>
     <row r="13" spans="2:8" s="9" customFormat="1" ht="20.45" customHeight="1">
-      <c r="B13" s="96" t="s">
+      <c r="B13" s="126" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="13" t="s">
@@ -3135,7 +3141,7 @@
       <c r="G13" s="34"/>
     </row>
     <row r="14" spans="2:8" s="9" customFormat="1" ht="20.45" customHeight="1">
-      <c r="B14" s="96"/>
+      <c r="B14" s="126"/>
       <c r="C14" s="23" t="s">
         <v>36</v>
       </c>
@@ -3147,7 +3153,7 @@
       <c r="G14" s="34"/>
     </row>
     <row r="15" spans="2:8" s="9" customFormat="1" ht="20.45" customHeight="1">
-      <c r="B15" s="96"/>
+      <c r="B15" s="126"/>
       <c r="C15" s="24" t="s">
         <v>37</v>
       </c>
@@ -3159,7 +3165,7 @@
       <c r="G15" s="34"/>
     </row>
     <row r="16" spans="2:8" s="9" customFormat="1" ht="20.45" customHeight="1">
-      <c r="B16" s="96"/>
+      <c r="B16" s="126"/>
       <c r="C16" s="54" t="s">
         <v>29</v>
       </c>
@@ -3171,7 +3177,7 @@
       <c r="G16" s="34"/>
     </row>
     <row r="17" spans="2:7" s="9" customFormat="1" ht="20.45" customHeight="1">
-      <c r="B17" s="96"/>
+      <c r="B17" s="126"/>
       <c r="C17" s="25"/>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
@@ -3179,7 +3185,7 @@
       <c r="G17" s="34"/>
     </row>
     <row r="18" spans="2:7" s="9" customFormat="1" ht="20.45" customHeight="1">
-      <c r="B18" s="96"/>
+      <c r="B18" s="126"/>
       <c r="C18" s="27"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
@@ -3218,21 +3224,21 @@
   <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B103" sqref="B103"/>
+      <selection pane="bottomLeft" activeCell="G46" sqref="G46:H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="13.5" thickBottom="1"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="113"/>
-    <col min="2" max="2" width="10.85546875" style="104"/>
-    <col min="3" max="3" width="11.5703125" style="113" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="109"/>
+    <col min="2" max="2" width="10.85546875" style="100"/>
+    <col min="3" max="3" width="11.5703125" style="109" customWidth="1"/>
     <col min="4" max="4" width="42" style="87" customWidth="1"/>
     <col min="5" max="5" width="67.42578125" style="87" customWidth="1"/>
     <col min="6" max="6" width="35.7109375" style="87" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" style="124" customWidth="1"/>
-    <col min="8" max="8" width="13" style="115" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="120" customWidth="1"/>
+    <col min="8" max="8" width="13" style="111" customWidth="1"/>
     <col min="9" max="11" width="10.85546875" style="84"/>
     <col min="12" max="12" width="10.85546875" style="87"/>
     <col min="13" max="13" width="21" style="86" customWidth="1"/>
@@ -3241,22 +3247,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="26.25" thickBot="1">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="97" t="s">
+      <c r="C1" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="98" t="s">
+      <c r="D1" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="98" t="s">
+      <c r="E1" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="98" t="s">
+      <c r="F1" s="94" t="s">
         <v>19</v>
       </c>
       <c r="G1" s="49" t="s">
@@ -3277,20 +3283,20 @@
       <c r="L1" s="49" t="s">
         <v>271</v>
       </c>
-      <c r="M1" s="99" t="s">
+      <c r="M1" s="95" t="s">
         <v>285</v>
       </c>
       <c r="N1" s="43"/>
     </row>
     <row r="2" spans="1:18" ht="26.25" thickBot="1">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="96" t="s">
         <v>291</v>
       </c>
-      <c r="B2" s="100" t="str">
+      <c r="B2" s="96" t="str">
         <f>_xlfn.CONCAT("131_", TEXT(ROW()-1, "0000"))</f>
         <v>131_0001</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="C2" s="96" t="s">
         <v>264</v>
       </c>
       <c r="D2" s="85" t="s">
@@ -3299,13 +3305,13 @@
       <c r="E2" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="101" t="s">
+      <c r="F2" s="97" t="s">
         <v>192</v>
       </c>
       <c r="G2" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="102">
+      <c r="H2" s="98">
         <v>7.3</v>
       </c>
       <c r="I2" s="87" t="s">
@@ -3321,14 +3327,14 @@
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" ht="26.25" hidden="1" thickBot="1">
-      <c r="A3" s="100" t="s">
+      <c r="A3" s="96" t="s">
         <v>292</v>
       </c>
-      <c r="B3" s="100" t="str">
+      <c r="B3" s="96" t="str">
         <f t="shared" ref="B3:B66" si="0">_xlfn.CONCAT("131_", TEXT(ROW()-1, "0000"))</f>
         <v>131_0002</v>
       </c>
-      <c r="C3" s="100" t="s">
+      <c r="C3" s="96" t="s">
         <v>264</v>
       </c>
       <c r="D3" s="85" t="s">
@@ -3337,11 +3343,11 @@
       <c r="E3" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="101" t="s">
+      <c r="F3" s="97" t="s">
         <v>193</v>
       </c>
-      <c r="G3" s="103"/>
-      <c r="H3" s="102"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="98"/>
       <c r="I3" s="87" t="s">
         <v>31</v>
       </c>
@@ -3357,14 +3363,14 @@
       <c r="N3" s="43"/>
     </row>
     <row r="4" spans="1:18" ht="39" thickBot="1">
-      <c r="A4" s="100" t="s">
+      <c r="A4" s="96" t="s">
         <v>293</v>
       </c>
-      <c r="B4" s="100" t="str">
+      <c r="B4" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0003</v>
       </c>
-      <c r="C4" s="104" t="s">
+      <c r="C4" s="100" t="s">
         <v>264</v>
       </c>
       <c r="D4" s="85" t="s">
@@ -3373,14 +3379,14 @@
       <c r="E4" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="101" t="s">
+      <c r="F4" s="97" t="s">
         <v>194</v>
       </c>
       <c r="G4" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="H4" s="100" t="s">
-        <v>427</v>
+      <c r="H4" s="96" t="s">
+        <v>467</v>
       </c>
       <c r="I4" s="87" t="s">
         <v>31</v>
@@ -3391,14 +3397,14 @@
       <c r="N4" s="43"/>
     </row>
     <row r="5" spans="1:18" ht="26.25" thickBot="1">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="96" t="s">
         <v>294</v>
       </c>
-      <c r="B5" s="100" t="str">
+      <c r="B5" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0004</v>
       </c>
-      <c r="C5" s="104" t="s">
+      <c r="C5" s="100" t="s">
         <v>264</v>
       </c>
       <c r="D5" s="85" t="s">
@@ -3407,13 +3413,13 @@
       <c r="E5" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="101" t="s">
+      <c r="F5" s="97" t="s">
         <v>195</v>
       </c>
       <c r="G5" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="H5" s="100" t="s">
+      <c r="H5" s="96" t="s">
         <v>428</v>
       </c>
       <c r="I5" s="87" t="s">
@@ -3425,14 +3431,14 @@
       <c r="N5" s="43"/>
     </row>
     <row r="6" spans="1:18" ht="26.25" thickBot="1">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="96" t="s">
         <v>295</v>
       </c>
-      <c r="B6" s="100" t="str">
+      <c r="B6" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0005</v>
       </c>
-      <c r="C6" s="104" t="s">
+      <c r="C6" s="100" t="s">
         <v>264</v>
       </c>
       <c r="D6" s="85" t="s">
@@ -3441,13 +3447,13 @@
       <c r="E6" s="85" t="s">
         <v>426</v>
       </c>
-      <c r="F6" s="101" t="s">
+      <c r="F6" s="97" t="s">
         <v>196</v>
       </c>
       <c r="G6" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="H6" s="100" t="s">
+      <c r="H6" s="96" t="s">
         <v>427</v>
       </c>
       <c r="I6" s="87" t="s">
@@ -3459,14 +3465,14 @@
       <c r="N6" s="43"/>
     </row>
     <row r="7" spans="1:18" s="46" customFormat="1" ht="39" hidden="1" thickBot="1">
-      <c r="A7" s="100" t="s">
+      <c r="A7" s="96" t="s">
         <v>296</v>
       </c>
-      <c r="B7" s="100" t="str">
+      <c r="B7" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0006</v>
       </c>
-      <c r="C7" s="105" t="s">
+      <c r="C7" s="101" t="s">
         <v>264</v>
       </c>
       <c r="D7" s="85" t="s">
@@ -3475,13 +3481,13 @@
       <c r="E7" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="106" t="s">
+      <c r="F7" s="102" t="s">
         <v>197</v>
       </c>
       <c r="G7" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="102">
+      <c r="H7" s="98">
         <v>7.1</v>
       </c>
       <c r="I7" s="87" t="s">
@@ -3500,14 +3506,14 @@
       <c r="N7" s="43"/>
     </row>
     <row r="8" spans="1:18" s="46" customFormat="1" ht="26.25" thickBot="1">
-      <c r="A8" s="100" t="s">
+      <c r="A8" s="96" t="s">
         <v>297</v>
       </c>
-      <c r="B8" s="100" t="str">
+      <c r="B8" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0007</v>
       </c>
-      <c r="C8" s="105" t="s">
+      <c r="C8" s="101" t="s">
         <v>265</v>
       </c>
       <c r="D8" s="85" t="s">
@@ -3516,13 +3522,13 @@
       <c r="E8" s="85" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="106" t="s">
+      <c r="F8" s="102" t="s">
         <v>198</v>
       </c>
       <c r="G8" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="H8" s="102" t="s">
+      <c r="H8" s="98" t="s">
         <v>272</v>
       </c>
       <c r="I8" s="87" t="s">
@@ -3537,14 +3543,14 @@
       <c r="N8" s="43"/>
     </row>
     <row r="9" spans="1:18" ht="26.25" hidden="1" thickBot="1">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="96" t="s">
         <v>298</v>
       </c>
-      <c r="B9" s="100" t="str">
+      <c r="B9" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0008</v>
       </c>
-      <c r="C9" s="104" t="s">
+      <c r="C9" s="100" t="s">
         <v>264</v>
       </c>
       <c r="D9" s="85" t="s">
@@ -3553,13 +3559,13 @@
       <c r="E9" s="85" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="101" t="s">
+      <c r="F9" s="97" t="s">
         <v>199</v>
       </c>
       <c r="G9" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="H9" s="102">
+      <c r="H9" s="98">
         <v>4.2</v>
       </c>
       <c r="I9" s="87" t="s">
@@ -3577,14 +3583,14 @@
       </c>
     </row>
     <row r="10" spans="1:18" ht="26.25" thickBot="1">
-      <c r="A10" s="100" t="s">
+      <c r="A10" s="96" t="s">
         <v>299</v>
       </c>
-      <c r="B10" s="100" t="str">
+      <c r="B10" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0009</v>
       </c>
-      <c r="C10" s="104" t="s">
+      <c r="C10" s="100" t="s">
         <v>266</v>
       </c>
       <c r="D10" s="85" t="s">
@@ -3593,13 +3599,13 @@
       <c r="E10" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="101" t="s">
+      <c r="F10" s="97" t="s">
         <v>200</v>
       </c>
       <c r="G10" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="102" t="s">
+      <c r="H10" s="98" t="s">
         <v>273</v>
       </c>
       <c r="I10" s="87" t="s">
@@ -3612,14 +3618,14 @@
       </c>
     </row>
     <row r="11" spans="1:18" ht="26.25" thickBot="1">
-      <c r="A11" s="100" t="s">
+      <c r="A11" s="96" t="s">
         <v>300</v>
       </c>
-      <c r="B11" s="100" t="str">
+      <c r="B11" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0010</v>
       </c>
-      <c r="C11" s="104" t="s">
+      <c r="C11" s="100" t="s">
         <v>266</v>
       </c>
       <c r="D11" s="85" t="s">
@@ -3628,13 +3634,13 @@
       <c r="E11" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="101" t="s">
+      <c r="F11" s="97" t="s">
         <v>201</v>
       </c>
       <c r="G11" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="H11" s="100" t="s">
+      <c r="H11" s="96" t="s">
         <v>404</v>
       </c>
       <c r="I11" s="87" t="s">
@@ -3645,20 +3651,20 @@
       <c r="L11" s="85" t="s">
         <v>267</v>
       </c>
-      <c r="M11" s="125" t="s">
+      <c r="M11" s="121" t="s">
         <v>429</v>
       </c>
       <c r="N11" s="43"/>
     </row>
     <row r="12" spans="1:18" ht="39" hidden="1" thickBot="1">
-      <c r="A12" s="100" t="s">
+      <c r="A12" s="96" t="s">
         <v>301</v>
       </c>
-      <c r="B12" s="100" t="str">
+      <c r="B12" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0011</v>
       </c>
-      <c r="C12" s="100" t="s">
+      <c r="C12" s="96" t="s">
         <v>264</v>
       </c>
       <c r="D12" s="85" t="s">
@@ -3667,13 +3673,13 @@
       <c r="E12" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="107" t="s">
+      <c r="F12" s="103" t="s">
         <v>202</v>
       </c>
       <c r="G12" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="H12" s="102">
+      <c r="H12" s="98">
         <v>4.2</v>
       </c>
       <c r="I12" s="87" t="s">
@@ -3692,14 +3698,14 @@
       <c r="N12" s="43"/>
     </row>
     <row r="13" spans="1:18" s="46" customFormat="1" ht="26.25" hidden="1" thickBot="1">
-      <c r="A13" s="100" t="s">
+      <c r="A13" s="96" t="s">
         <v>302</v>
       </c>
-      <c r="B13" s="100" t="str">
+      <c r="B13" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0012</v>
       </c>
-      <c r="C13" s="105" t="s">
+      <c r="C13" s="101" t="s">
         <v>264</v>
       </c>
       <c r="D13" s="85" t="s">
@@ -3708,13 +3714,13 @@
       <c r="E13" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="101" t="s">
+      <c r="F13" s="97" t="s">
         <v>203</v>
       </c>
       <c r="G13" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="H13" s="102">
+      <c r="H13" s="98">
         <v>4.2</v>
       </c>
       <c r="I13" s="87" t="s">
@@ -3733,27 +3739,27 @@
       <c r="N13" s="43"/>
     </row>
     <row r="14" spans="1:18" s="46" customFormat="1" ht="26.25" hidden="1" thickBot="1">
-      <c r="A14" s="100" t="s">
+      <c r="A14" s="96" t="s">
         <v>303</v>
       </c>
-      <c r="B14" s="100" t="str">
+      <c r="B14" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0013</v>
       </c>
-      <c r="C14" s="105" t="s">
+      <c r="C14" s="101" t="s">
         <v>264</v>
       </c>
-      <c r="D14" s="101" t="s">
+      <c r="D14" s="97" t="s">
         <v>376</v>
       </c>
       <c r="E14" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="101" t="s">
+      <c r="F14" s="97" t="s">
         <v>204</v>
       </c>
       <c r="G14" s="85"/>
-      <c r="H14" s="102"/>
+      <c r="H14" s="98"/>
       <c r="I14" s="87" t="s">
         <v>31</v>
       </c>
@@ -3770,14 +3776,14 @@
       <c r="N14" s="43"/>
     </row>
     <row r="15" spans="1:18" ht="26.25" hidden="1" thickBot="1">
-      <c r="A15" s="100" t="s">
+      <c r="A15" s="96" t="s">
         <v>304</v>
       </c>
-      <c r="B15" s="100" t="str">
+      <c r="B15" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0014</v>
       </c>
-      <c r="C15" s="100" t="s">
+      <c r="C15" s="96" t="s">
         <v>264</v>
       </c>
       <c r="D15" s="85" t="s">
@@ -3786,13 +3792,13 @@
       <c r="E15" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="F15" s="108" t="s">
+      <c r="F15" s="104" t="s">
         <v>205</v>
       </c>
       <c r="G15" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="H15" s="102">
+      <c r="H15" s="98">
         <v>4.2</v>
       </c>
       <c r="I15" s="87" t="s">
@@ -3811,14 +3817,14 @@
       <c r="N15" s="43"/>
     </row>
     <row r="16" spans="1:18" s="46" customFormat="1" ht="26.25" hidden="1" thickBot="1">
-      <c r="A16" s="100" t="s">
+      <c r="A16" s="96" t="s">
         <v>305</v>
       </c>
-      <c r="B16" s="100" t="str">
+      <c r="B16" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0015</v>
       </c>
-      <c r="C16" s="102" t="s">
+      <c r="C16" s="98" t="s">
         <v>264</v>
       </c>
       <c r="D16" s="85" t="s">
@@ -3827,13 +3833,13 @@
       <c r="E16" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="109" t="s">
+      <c r="F16" s="105" t="s">
         <v>206</v>
       </c>
       <c r="G16" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="H16" s="102">
+      <c r="H16" s="98">
         <v>4.2</v>
       </c>
       <c r="I16" s="87" t="s">
@@ -3852,29 +3858,29 @@
       <c r="N16" s="43"/>
     </row>
     <row r="17" spans="1:14" ht="26.25" hidden="1" thickBot="1">
-      <c r="A17" s="100" t="s">
+      <c r="A17" s="96" t="s">
         <v>306</v>
       </c>
-      <c r="B17" s="100" t="str">
+      <c r="B17" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0016</v>
       </c>
-      <c r="C17" s="100" t="s">
+      <c r="C17" s="96" t="s">
         <v>264</v>
       </c>
-      <c r="D17" s="108" t="s">
+      <c r="D17" s="104" t="s">
         <v>123</v>
       </c>
       <c r="E17" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="108" t="s">
+      <c r="F17" s="104" t="s">
         <v>207</v>
       </c>
       <c r="G17" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="H17" s="102">
+      <c r="H17" s="98">
         <v>4.2</v>
       </c>
       <c r="I17" s="87" t="s">
@@ -3893,14 +3899,14 @@
       <c r="N17" s="43"/>
     </row>
     <row r="18" spans="1:14" ht="26.25" hidden="1" thickBot="1">
-      <c r="A18" s="100" t="s">
+      <c r="A18" s="96" t="s">
         <v>307</v>
       </c>
-      <c r="B18" s="100" t="str">
+      <c r="B18" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0017</v>
       </c>
-      <c r="C18" s="100" t="s">
+      <c r="C18" s="96" t="s">
         <v>264</v>
       </c>
       <c r="D18" s="85" t="s">
@@ -3909,13 +3915,13 @@
       <c r="E18" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="101" t="s">
+      <c r="F18" s="97" t="s">
         <v>208</v>
       </c>
       <c r="G18" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="H18" s="102">
+      <c r="H18" s="98">
         <v>4.2</v>
       </c>
       <c r="I18" s="87" t="s">
@@ -3933,14 +3939,14 @@
       <c r="N18" s="43"/>
     </row>
     <row r="19" spans="1:14" ht="39" hidden="1" thickBot="1">
-      <c r="A19" s="100" t="s">
+      <c r="A19" s="96" t="s">
         <v>308</v>
       </c>
-      <c r="B19" s="100" t="str">
+      <c r="B19" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0018</v>
       </c>
-      <c r="C19" s="104" t="s">
+      <c r="C19" s="100" t="s">
         <v>265</v>
       </c>
       <c r="D19" s="85" t="s">
@@ -3949,13 +3955,13 @@
       <c r="E19" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="101" t="s">
+      <c r="F19" s="97" t="s">
         <v>209</v>
       </c>
       <c r="G19" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H19" s="102" t="s">
+      <c r="H19" s="98" t="s">
         <v>381</v>
       </c>
       <c r="I19" s="87" t="s">
@@ -3973,14 +3979,14 @@
       <c r="N19" s="43"/>
     </row>
     <row r="20" spans="1:14" ht="26.25" thickBot="1">
-      <c r="A20" s="100" t="s">
+      <c r="A20" s="96" t="s">
         <v>309</v>
       </c>
-      <c r="B20" s="100" t="str">
+      <c r="B20" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0019</v>
       </c>
-      <c r="C20" s="100" t="s">
+      <c r="C20" s="96" t="s">
         <v>264</v>
       </c>
       <c r="D20" s="85" t="s">
@@ -3989,13 +3995,13 @@
       <c r="E20" s="85" t="s">
         <v>55</v>
       </c>
-      <c r="F20" s="101" t="s">
+      <c r="F20" s="97" t="s">
         <v>210</v>
       </c>
       <c r="G20" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H20" s="102" t="s">
+      <c r="H20" s="98" t="s">
         <v>274</v>
       </c>
       <c r="I20" s="87" t="s">
@@ -4007,14 +4013,14 @@
       <c r="N20" s="43"/>
     </row>
     <row r="21" spans="1:14" ht="39" thickBot="1">
-      <c r="A21" s="100" t="s">
+      <c r="A21" s="96" t="s">
         <v>310</v>
       </c>
-      <c r="B21" s="100" t="str">
+      <c r="B21" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0020</v>
       </c>
-      <c r="C21" s="100" t="s">
+      <c r="C21" s="96" t="s">
         <v>264</v>
       </c>
       <c r="D21" s="85" t="s">
@@ -4023,13 +4029,13 @@
       <c r="E21" s="85" t="s">
         <v>385</v>
       </c>
-      <c r="F21" s="101" t="s">
+      <c r="F21" s="97" t="s">
         <v>211</v>
       </c>
       <c r="G21" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="H21" s="100" t="s">
+      <c r="H21" s="96" t="s">
         <v>430</v>
       </c>
       <c r="I21" s="87" t="s">
@@ -4047,14 +4053,14 @@
       <c r="N21" s="43"/>
     </row>
     <row r="22" spans="1:14" ht="39" thickBot="1">
-      <c r="A22" s="100" t="s">
+      <c r="A22" s="96" t="s">
         <v>311</v>
       </c>
-      <c r="B22" s="100" t="str">
+      <c r="B22" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0021</v>
       </c>
-      <c r="C22" s="100" t="s">
+      <c r="C22" s="96" t="s">
         <v>266</v>
       </c>
       <c r="D22" s="85" t="s">
@@ -4063,13 +4069,13 @@
       <c r="E22" s="85" t="s">
         <v>282</v>
       </c>
-      <c r="F22" s="101" t="s">
+      <c r="F22" s="97" t="s">
         <v>212</v>
       </c>
       <c r="G22" s="85" t="s">
         <v>405</v>
       </c>
-      <c r="H22" s="102"/>
+      <c r="H22" s="98"/>
       <c r="I22" s="87" t="s">
         <v>31</v>
       </c>
@@ -4082,14 +4088,14 @@
       <c r="N22" s="43"/>
     </row>
     <row r="23" spans="1:14" ht="51.75" thickBot="1">
-      <c r="A23" s="100" t="s">
+      <c r="A23" s="96" t="s">
         <v>312</v>
       </c>
-      <c r="B23" s="100" t="str">
+      <c r="B23" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0022</v>
       </c>
-      <c r="C23" s="105" t="s">
+      <c r="C23" s="101" t="s">
         <v>266</v>
       </c>
       <c r="D23" s="85" t="s">
@@ -4098,13 +4104,13 @@
       <c r="E23" s="85" t="s">
         <v>283</v>
       </c>
-      <c r="F23" s="101" t="s">
+      <c r="F23" s="97" t="s">
         <v>213</v>
       </c>
       <c r="G23" s="85" t="s">
         <v>405</v>
       </c>
-      <c r="H23" s="102"/>
+      <c r="H23" s="98"/>
       <c r="I23" s="87" t="s">
         <v>31</v>
       </c>
@@ -4117,29 +4123,29 @@
       <c r="N23" s="43"/>
     </row>
     <row r="24" spans="1:14" ht="26.25" thickBot="1">
-      <c r="A24" s="100" t="s">
+      <c r="A24" s="96" t="s">
         <v>313</v>
       </c>
-      <c r="B24" s="100" t="str">
+      <c r="B24" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0023</v>
       </c>
-      <c r="C24" s="104" t="s">
+      <c r="C24" s="100" t="s">
         <v>266</v>
       </c>
       <c r="D24" s="85" t="s">
         <v>130</v>
       </c>
-      <c r="E24" s="110" t="s">
+      <c r="E24" s="106" t="s">
         <v>288</v>
       </c>
-      <c r="F24" s="101" t="s">
+      <c r="F24" s="97" t="s">
         <v>214</v>
       </c>
       <c r="G24" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="H24" s="102" t="s">
+      <c r="H24" s="98" t="s">
         <v>275</v>
       </c>
       <c r="I24" s="87" t="s">
@@ -4157,29 +4163,29 @@
       <c r="N24" s="43"/>
     </row>
     <row r="25" spans="1:14" ht="39" thickBot="1">
-      <c r="A25" s="100" t="s">
+      <c r="A25" s="96" t="s">
         <v>314</v>
       </c>
-      <c r="B25" s="100" t="str">
+      <c r="B25" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0024</v>
       </c>
-      <c r="C25" s="104" t="s">
+      <c r="C25" s="100" t="s">
         <v>266</v>
       </c>
-      <c r="D25" s="101" t="s">
+      <c r="D25" s="97" t="s">
         <v>182</v>
       </c>
       <c r="E25" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="101" t="s">
+      <c r="F25" s="97" t="s">
         <v>215</v>
       </c>
-      <c r="G25" s="126" t="s">
+      <c r="G25" s="122" t="s">
         <v>405</v>
       </c>
-      <c r="H25" s="102"/>
+      <c r="H25" s="98"/>
       <c r="I25" s="87" t="s">
         <v>31</v>
       </c>
@@ -4192,14 +4198,14 @@
       <c r="N25" s="43"/>
     </row>
     <row r="26" spans="1:14" ht="26.25" thickBot="1">
-      <c r="A26" s="100" t="s">
+      <c r="A26" s="96" t="s">
         <v>315</v>
       </c>
-      <c r="B26" s="100" t="str">
+      <c r="B26" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0025</v>
       </c>
-      <c r="C26" s="104" t="s">
+      <c r="C26" s="100" t="s">
         <v>266</v>
       </c>
       <c r="D26" s="85" t="s">
@@ -4208,13 +4214,13 @@
       <c r="E26" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="F26" s="101" t="s">
+      <c r="F26" s="97" t="s">
         <v>216</v>
       </c>
       <c r="G26" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H26" s="102" t="s">
+      <c r="H26" s="98" t="s">
         <v>276</v>
       </c>
       <c r="I26" s="87" t="s">
@@ -4226,14 +4232,14 @@
       <c r="N26" s="43"/>
     </row>
     <row r="27" spans="1:14" ht="26.25" thickBot="1">
-      <c r="A27" s="100" t="s">
+      <c r="A27" s="96" t="s">
         <v>316</v>
       </c>
-      <c r="B27" s="100" t="str">
+      <c r="B27" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0026</v>
       </c>
-      <c r="C27" s="104" t="s">
+      <c r="C27" s="100" t="s">
         <v>266</v>
       </c>
       <c r="D27" s="85" t="s">
@@ -4242,13 +4248,13 @@
       <c r="E27" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="F27" s="101" t="s">
+      <c r="F27" s="97" t="s">
         <v>217</v>
       </c>
       <c r="G27" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H27" s="102" t="s">
+      <c r="H27" s="98" t="s">
         <v>276</v>
       </c>
       <c r="I27" s="87" t="s">
@@ -4260,29 +4266,29 @@
       <c r="N27" s="43"/>
     </row>
     <row r="28" spans="1:14" ht="39" thickBot="1">
-      <c r="A28" s="100" t="s">
+      <c r="A28" s="96" t="s">
         <v>317</v>
       </c>
-      <c r="B28" s="100" t="str">
+      <c r="B28" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0027</v>
       </c>
-      <c r="C28" s="100" t="s">
+      <c r="C28" s="96" t="s">
         <v>265</v>
       </c>
       <c r="D28" s="85" t="s">
         <v>133</v>
       </c>
-      <c r="E28" s="110" t="s">
+      <c r="E28" s="106" t="s">
         <v>386</v>
       </c>
-      <c r="F28" s="111" t="s">
+      <c r="F28" s="107" t="s">
         <v>406</v>
       </c>
       <c r="G28" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H28" s="100" t="s">
+      <c r="H28" s="96" t="s">
         <v>435</v>
       </c>
       <c r="I28" s="87" t="s">
@@ -4300,14 +4306,14 @@
       <c r="N28" s="43"/>
     </row>
     <row r="29" spans="1:14" ht="26.25" hidden="1" thickBot="1">
-      <c r="A29" s="100" t="s">
+      <c r="A29" s="96" t="s">
         <v>318</v>
       </c>
-      <c r="B29" s="100" t="str">
+      <c r="B29" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0028</v>
       </c>
-      <c r="C29" s="104" t="s">
+      <c r="C29" s="100" t="s">
         <v>264</v>
       </c>
       <c r="D29" s="85" t="s">
@@ -4316,13 +4322,13 @@
       <c r="E29" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="F29" s="101" t="s">
+      <c r="F29" s="97" t="s">
         <v>218</v>
       </c>
       <c r="G29" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="H29" s="100" t="s">
+      <c r="H29" s="96" t="s">
         <v>436</v>
       </c>
       <c r="I29" s="87" t="s">
@@ -4340,29 +4346,29 @@
       <c r="N29" s="43"/>
     </row>
     <row r="30" spans="1:14" s="46" customFormat="1" ht="39" hidden="1" thickBot="1">
-      <c r="A30" s="100" t="s">
+      <c r="A30" s="96" t="s">
         <v>319</v>
       </c>
-      <c r="B30" s="100" t="str">
+      <c r="B30" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0029</v>
       </c>
-      <c r="C30" s="102" t="s">
+      <c r="C30" s="98" t="s">
         <v>265</v>
       </c>
-      <c r="D30" s="101" t="s">
+      <c r="D30" s="97" t="s">
         <v>135</v>
       </c>
       <c r="E30" s="85" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="101" t="s">
+      <c r="F30" s="97" t="s">
         <v>219</v>
       </c>
       <c r="G30" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H30" s="102">
+      <c r="H30" s="98">
         <v>4.2</v>
       </c>
       <c r="I30" s="87" t="s">
@@ -4381,29 +4387,29 @@
       <c r="N30" s="43"/>
     </row>
     <row r="31" spans="1:14" s="46" customFormat="1" ht="39" thickBot="1">
-      <c r="A31" s="100" t="s">
+      <c r="A31" s="96" t="s">
         <v>320</v>
       </c>
-      <c r="B31" s="100" t="str">
+      <c r="B31" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0030</v>
       </c>
-      <c r="C31" s="105" t="s">
+      <c r="C31" s="101" t="s">
         <v>264</v>
       </c>
-      <c r="D31" s="112" t="s">
+      <c r="D31" s="108" t="s">
         <v>377</v>
       </c>
       <c r="E31" s="85" t="s">
         <v>390</v>
       </c>
-      <c r="F31" s="101" t="s">
+      <c r="F31" s="97" t="s">
         <v>220</v>
       </c>
       <c r="G31" s="85" t="s">
         <v>405</v>
       </c>
-      <c r="H31" s="102"/>
+      <c r="H31" s="98"/>
       <c r="I31" s="87" t="s">
         <v>31</v>
       </c>
@@ -4420,29 +4426,29 @@
       <c r="N31" s="43"/>
     </row>
     <row r="32" spans="1:14" ht="26.25" hidden="1" thickBot="1">
-      <c r="A32" s="100" t="s">
+      <c r="A32" s="96" t="s">
         <v>321</v>
       </c>
-      <c r="B32" s="100" t="str">
+      <c r="B32" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0031</v>
       </c>
-      <c r="C32" s="104" t="s">
+      <c r="C32" s="100" t="s">
         <v>264</v>
       </c>
-      <c r="D32" s="112" t="s">
+      <c r="D32" s="108" t="s">
         <v>136</v>
       </c>
       <c r="E32" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="F32" s="101" t="s">
+      <c r="F32" s="97" t="s">
         <v>221</v>
       </c>
       <c r="G32" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="H32" s="105">
+      <c r="H32" s="101">
         <v>4.2</v>
       </c>
       <c r="I32" s="84" t="s">
@@ -4460,29 +4466,29 @@
       <c r="N32" s="43"/>
     </row>
     <row r="33" spans="1:13" ht="26.25" hidden="1" thickBot="1">
-      <c r="A33" s="100" t="s">
+      <c r="A33" s="96" t="s">
         <v>322</v>
       </c>
-      <c r="B33" s="100" t="str">
+      <c r="B33" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0032</v>
       </c>
-      <c r="C33" s="113" t="s">
+      <c r="C33" s="109" t="s">
         <v>264</v>
       </c>
-      <c r="D33" s="112" t="s">
+      <c r="D33" s="108" t="s">
         <v>137</v>
       </c>
       <c r="E33" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="F33" s="114" t="s">
+      <c r="F33" s="110" t="s">
         <v>222</v>
       </c>
       <c r="G33" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="H33" s="115">
+      <c r="H33" s="111">
         <v>4.2</v>
       </c>
       <c r="I33" s="84" t="s">
@@ -4499,14 +4505,14 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="26.25" hidden="1" thickBot="1">
-      <c r="A34" s="100" t="s">
+      <c r="A34" s="96" t="s">
         <v>323</v>
       </c>
-      <c r="B34" s="100" t="str">
+      <c r="B34" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0033</v>
       </c>
-      <c r="C34" s="113" t="s">
+      <c r="C34" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D34" s="87" t="s">
@@ -4515,13 +4521,13 @@
       <c r="E34" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="F34" s="114" t="s">
+      <c r="F34" s="110" t="s">
         <v>223</v>
       </c>
       <c r="G34" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="H34" s="115">
+      <c r="H34" s="111">
         <v>4.2</v>
       </c>
       <c r="I34" s="84" t="s">
@@ -4538,14 +4544,14 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="26.25" hidden="1" thickBot="1">
-      <c r="A35" s="100" t="s">
+      <c r="A35" s="96" t="s">
         <v>324</v>
       </c>
-      <c r="B35" s="100" t="str">
+      <c r="B35" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0034</v>
       </c>
-      <c r="C35" s="113" t="s">
+      <c r="C35" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D35" s="87" t="s">
@@ -4554,13 +4560,13 @@
       <c r="E35" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="F35" s="114" t="s">
+      <c r="F35" s="110" t="s">
         <v>224</v>
       </c>
       <c r="G35" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="H35" s="115">
+      <c r="H35" s="111">
         <v>4.2</v>
       </c>
       <c r="I35" s="84" t="s">
@@ -4577,14 +4583,14 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="26.25" hidden="1" thickBot="1">
-      <c r="A36" s="100" t="s">
+      <c r="A36" s="96" t="s">
         <v>325</v>
       </c>
-      <c r="B36" s="100" t="str">
+      <c r="B36" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0035</v>
       </c>
-      <c r="C36" s="113" t="s">
+      <c r="C36" s="109" t="s">
         <v>265</v>
       </c>
       <c r="D36" s="85" t="s">
@@ -4593,7 +4599,7 @@
       <c r="E36" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="F36" s="114" t="s">
+      <c r="F36" s="110" t="s">
         <v>225</v>
       </c>
       <c r="G36" s="85"/>
@@ -4611,14 +4617,14 @@
       </c>
     </row>
     <row r="37" spans="1:13" ht="26.25" hidden="1" thickBot="1">
-      <c r="A37" s="100" t="s">
+      <c r="A37" s="96" t="s">
         <v>326</v>
       </c>
-      <c r="B37" s="100" t="str">
+      <c r="B37" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0036</v>
       </c>
-      <c r="C37" s="113" t="s">
+      <c r="C37" s="109" t="s">
         <v>265</v>
       </c>
       <c r="D37" s="85" t="s">
@@ -4627,7 +4633,7 @@
       <c r="E37" s="85" t="s">
         <v>66</v>
       </c>
-      <c r="F37" s="114" t="s">
+      <c r="F37" s="110" t="s">
         <v>225</v>
       </c>
       <c r="G37" s="85"/>
@@ -4645,14 +4651,14 @@
       </c>
     </row>
     <row r="38" spans="1:13" ht="26.25" hidden="1" thickBot="1">
-      <c r="A38" s="100" t="s">
+      <c r="A38" s="96" t="s">
         <v>327</v>
       </c>
-      <c r="B38" s="100" t="str">
+      <c r="B38" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0037</v>
       </c>
-      <c r="C38" s="113" t="s">
+      <c r="C38" s="109" t="s">
         <v>265</v>
       </c>
       <c r="D38" s="85" t="s">
@@ -4661,7 +4667,7 @@
       <c r="E38" s="85" t="s">
         <v>67</v>
       </c>
-      <c r="F38" s="114" t="s">
+      <c r="F38" s="110" t="s">
         <v>226</v>
       </c>
       <c r="G38" s="85"/>
@@ -4679,14 +4685,14 @@
       </c>
     </row>
     <row r="39" spans="1:13" ht="26.25" hidden="1" thickBot="1">
-      <c r="A39" s="100" t="s">
+      <c r="A39" s="96" t="s">
         <v>328</v>
       </c>
-      <c r="B39" s="100" t="str">
+      <c r="B39" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0038</v>
       </c>
-      <c r="C39" s="113" t="s">
+      <c r="C39" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D39" s="85" t="s">
@@ -4695,7 +4701,7 @@
       <c r="E39" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="F39" s="114" t="s">
+      <c r="F39" s="110" t="s">
         <v>227</v>
       </c>
       <c r="G39" s="85"/>
@@ -4713,14 +4719,14 @@
       </c>
     </row>
     <row r="40" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A40" s="100" t="s">
+      <c r="A40" s="96" t="s">
         <v>329</v>
       </c>
-      <c r="B40" s="100" t="str">
+      <c r="B40" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0039</v>
       </c>
-      <c r="C40" s="113" t="s">
+      <c r="C40" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D40" s="85" t="s">
@@ -4729,13 +4735,13 @@
       <c r="E40" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="F40" s="114" t="s">
+      <c r="F40" s="110" t="s">
         <v>228</v>
       </c>
       <c r="G40" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H40" s="102">
+      <c r="H40" s="98">
         <v>12.9</v>
       </c>
       <c r="I40" s="84" t="s">
@@ -4746,14 +4752,14 @@
       </c>
     </row>
     <row r="41" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A41" s="100" t="s">
+      <c r="A41" s="96" t="s">
         <v>330</v>
       </c>
-      <c r="B41" s="100" t="str">
+      <c r="B41" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0040</v>
       </c>
-      <c r="C41" s="113" t="s">
+      <c r="C41" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D41" s="85" t="s">
@@ -4762,13 +4768,13 @@
       <c r="E41" s="85" t="s">
         <v>70</v>
       </c>
-      <c r="F41" s="114" t="s">
+      <c r="F41" s="110" t="s">
         <v>229</v>
       </c>
       <c r="G41" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H41" s="102">
+      <c r="H41" s="98">
         <v>12.12</v>
       </c>
       <c r="I41" s="84" t="s">
@@ -4779,14 +4785,14 @@
       </c>
     </row>
     <row r="42" spans="1:13" ht="39" thickBot="1">
-      <c r="A42" s="100" t="s">
+      <c r="A42" s="96" t="s">
         <v>331</v>
       </c>
-      <c r="B42" s="100" t="str">
+      <c r="B42" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0041</v>
       </c>
-      <c r="C42" s="113" t="s">
+      <c r="C42" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D42" s="85" t="s">
@@ -4795,13 +4801,13 @@
       <c r="E42" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="F42" s="114" t="s">
+      <c r="F42" s="110" t="s">
         <v>230</v>
       </c>
       <c r="G42" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H42" s="102">
+      <c r="H42" s="98">
         <v>12.12</v>
       </c>
       <c r="I42" s="84" t="s">
@@ -4812,14 +4818,14 @@
       </c>
     </row>
     <row r="43" spans="1:13" ht="39" thickBot="1">
-      <c r="A43" s="100" t="s">
+      <c r="A43" s="96" t="s">
         <v>332</v>
       </c>
-      <c r="B43" s="100" t="str">
+      <c r="B43" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0042</v>
       </c>
-      <c r="C43" s="116" t="s">
+      <c r="C43" s="112" t="s">
         <v>266</v>
       </c>
       <c r="D43" s="85" t="s">
@@ -4828,13 +4834,13 @@
       <c r="E43" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="F43" s="114" t="s">
+      <c r="F43" s="110" t="s">
         <v>231</v>
       </c>
       <c r="G43" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="H43" s="100" t="s">
+      <c r="H43" s="96" t="s">
         <v>438</v>
       </c>
       <c r="I43" s="84" t="s">
@@ -4848,14 +4854,14 @@
       </c>
     </row>
     <row r="44" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A44" s="100" t="s">
+      <c r="A44" s="96" t="s">
         <v>333</v>
       </c>
-      <c r="B44" s="100" t="str">
+      <c r="B44" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0043</v>
       </c>
-      <c r="C44" s="113" t="s">
+      <c r="C44" s="109" t="s">
         <v>266</v>
       </c>
       <c r="D44" s="85" t="s">
@@ -4864,13 +4870,13 @@
       <c r="E44" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="F44" s="114" t="s">
+      <c r="F44" s="110" t="s">
         <v>232</v>
       </c>
       <c r="G44" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H44" s="127">
+      <c r="H44" s="98">
         <v>12.1</v>
       </c>
       <c r="I44" s="84" t="s">
@@ -4881,14 +4887,14 @@
       </c>
     </row>
     <row r="45" spans="1:13" ht="26.25" hidden="1" thickBot="1">
-      <c r="A45" s="100" t="s">
+      <c r="A45" s="96" t="s">
         <v>334</v>
       </c>
-      <c r="B45" s="100" t="str">
+      <c r="B45" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0044</v>
       </c>
-      <c r="C45" s="113" t="s">
+      <c r="C45" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D45" s="85" t="s">
@@ -4897,13 +4903,13 @@
       <c r="E45" s="85" t="s">
         <v>74</v>
       </c>
-      <c r="F45" s="114" t="s">
+      <c r="F45" s="110" t="s">
         <v>233</v>
       </c>
       <c r="G45" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H45" s="127">
+      <c r="H45" s="98">
         <v>4.2</v>
       </c>
       <c r="I45" s="84" t="s">
@@ -4920,14 +4926,14 @@
       </c>
     </row>
     <row r="46" spans="1:13" ht="39" thickBot="1">
-      <c r="A46" s="100" t="s">
+      <c r="A46" s="96" t="s">
         <v>335</v>
       </c>
-      <c r="B46" s="100" t="str">
+      <c r="B46" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0045</v>
       </c>
-      <c r="C46" s="113" t="s">
+      <c r="C46" s="109" t="s">
         <v>266</v>
       </c>
       <c r="D46" s="85" t="s">
@@ -4936,11 +4942,14 @@
       <c r="E46" s="85" t="s">
         <v>75</v>
       </c>
-      <c r="F46" s="114" t="s">
+      <c r="F46" s="110" t="s">
         <v>234</v>
       </c>
-      <c r="G46" s="85" t="s">
-        <v>405</v>
+      <c r="G46" s="115" t="s">
+        <v>263</v>
+      </c>
+      <c r="H46" s="127" t="s">
+        <v>471</v>
       </c>
       <c r="I46" s="84" t="s">
         <v>31</v>
@@ -4953,14 +4962,14 @@
       </c>
     </row>
     <row r="47" spans="1:13" ht="26.25" hidden="1" thickBot="1">
-      <c r="A47" s="100" t="s">
+      <c r="A47" s="96" t="s">
         <v>336</v>
       </c>
-      <c r="B47" s="100" t="str">
+      <c r="B47" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0046</v>
       </c>
-      <c r="C47" s="113" t="s">
+      <c r="C47" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D47" s="85" t="s">
@@ -4969,7 +4978,7 @@
       <c r="E47" s="85" t="s">
         <v>76</v>
       </c>
-      <c r="F47" s="114" t="s">
+      <c r="F47" s="110" t="s">
         <v>235</v>
       </c>
       <c r="G47" s="85"/>
@@ -4987,14 +4996,14 @@
       </c>
     </row>
     <row r="48" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A48" s="100" t="s">
+      <c r="A48" s="96" t="s">
         <v>337</v>
       </c>
-      <c r="B48" s="100" t="str">
+      <c r="B48" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0047</v>
       </c>
-      <c r="C48" s="113" t="s">
+      <c r="C48" s="109" t="s">
         <v>266</v>
       </c>
       <c r="D48" s="85" t="s">
@@ -5003,13 +5012,13 @@
       <c r="E48" s="85" t="s">
         <v>77</v>
       </c>
-      <c r="F48" s="114" t="s">
+      <c r="F48" s="110" t="s">
         <v>236</v>
       </c>
       <c r="G48" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H48" s="100" t="s">
+      <c r="H48" s="96" t="s">
         <v>439</v>
       </c>
       <c r="I48" s="84" t="s">
@@ -5020,14 +5029,14 @@
       </c>
     </row>
     <row r="49" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A49" s="100" t="s">
+      <c r="A49" s="96" t="s">
         <v>338</v>
       </c>
-      <c r="B49" s="100" t="str">
+      <c r="B49" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0048</v>
       </c>
-      <c r="C49" s="113" t="s">
+      <c r="C49" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D49" s="85" t="s">
@@ -5036,11 +5045,14 @@
       <c r="E49" s="85" t="s">
         <v>78</v>
       </c>
-      <c r="F49" s="114" t="s">
+      <c r="F49" s="110" t="s">
         <v>237</v>
       </c>
       <c r="G49" s="85" t="s">
-        <v>405</v>
+        <v>263</v>
+      </c>
+      <c r="H49" s="109" t="s">
+        <v>470</v>
       </c>
       <c r="I49" s="84" t="s">
         <v>31</v>
@@ -5053,14 +5065,14 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="39" thickBot="1">
-      <c r="A50" s="100" t="s">
+      <c r="A50" s="96" t="s">
         <v>339</v>
       </c>
-      <c r="B50" s="100" t="str">
+      <c r="B50" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0049</v>
       </c>
-      <c r="C50" s="113" t="s">
+      <c r="C50" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D50" s="85" t="s">
@@ -5069,11 +5081,14 @@
       <c r="E50" s="85" t="s">
         <v>79</v>
       </c>
-      <c r="F50" s="114" t="s">
+      <c r="F50" s="110" t="s">
         <v>238</v>
       </c>
       <c r="G50" s="85" t="s">
-        <v>405</v>
+        <v>263</v>
+      </c>
+      <c r="H50" s="109" t="s">
+        <v>470</v>
       </c>
       <c r="I50" s="84" t="s">
         <v>31</v>
@@ -5086,14 +5101,14 @@
       </c>
     </row>
     <row r="51" spans="1:13" ht="39" hidden="1" thickBot="1">
-      <c r="A51" s="100" t="s">
+      <c r="A51" s="96" t="s">
         <v>340</v>
       </c>
-      <c r="B51" s="100" t="str">
+      <c r="B51" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0050</v>
       </c>
-      <c r="C51" s="113" t="s">
+      <c r="C51" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D51" s="85" t="s">
@@ -5102,13 +5117,13 @@
       <c r="E51" s="85" t="s">
         <v>80</v>
       </c>
-      <c r="F51" s="114" t="s">
+      <c r="F51" s="110" t="s">
         <v>239</v>
       </c>
       <c r="G51" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H51" s="102" t="s">
+      <c r="H51" s="98" t="s">
         <v>277</v>
       </c>
       <c r="I51" s="84" t="s">
@@ -5125,14 +5140,14 @@
       </c>
     </row>
     <row r="52" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A52" s="100" t="s">
+      <c r="A52" s="96" t="s">
         <v>341</v>
       </c>
-      <c r="B52" s="100" t="str">
+      <c r="B52" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0051</v>
       </c>
-      <c r="C52" s="113" t="s">
+      <c r="C52" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D52" s="85" t="s">
@@ -5141,13 +5156,13 @@
       <c r="E52" s="85" t="s">
         <v>81</v>
       </c>
-      <c r="F52" s="114" t="s">
+      <c r="F52" s="110" t="s">
         <v>240</v>
       </c>
       <c r="G52" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="H52" s="100" t="s">
+      <c r="H52" s="96" t="s">
         <v>440</v>
       </c>
       <c r="I52" s="84" t="s">
@@ -5158,14 +5173,14 @@
       </c>
     </row>
     <row r="53" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A53" s="100" t="s">
+      <c r="A53" s="96" t="s">
         <v>342</v>
       </c>
-      <c r="B53" s="100" t="str">
+      <c r="B53" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0052</v>
       </c>
-      <c r="C53" s="113" t="s">
+      <c r="C53" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D53" s="85" t="s">
@@ -5174,11 +5189,14 @@
       <c r="E53" s="85" t="s">
         <v>421</v>
       </c>
-      <c r="F53" s="114" t="s">
+      <c r="F53" s="110" t="s">
         <v>241</v>
       </c>
-      <c r="G53" s="85" t="s">
-        <v>405</v>
+      <c r="G53" s="115" t="s">
+        <v>263</v>
+      </c>
+      <c r="H53" s="127" t="s">
+        <v>471</v>
       </c>
       <c r="I53" s="84" t="s">
         <v>31</v>
@@ -5191,14 +5209,14 @@
       </c>
     </row>
     <row r="54" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A54" s="100" t="s">
+      <c r="A54" s="96" t="s">
         <v>343</v>
       </c>
-      <c r="B54" s="100" t="str">
+      <c r="B54" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0053</v>
       </c>
-      <c r="C54" s="113" t="s">
+      <c r="C54" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D54" s="85" t="s">
@@ -5207,13 +5225,13 @@
       <c r="E54" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="F54" s="114" t="s">
+      <c r="F54" s="110" t="s">
         <v>254</v>
       </c>
       <c r="G54" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="H54" s="102" t="s">
+      <c r="H54" s="98" t="s">
         <v>382</v>
       </c>
       <c r="I54" s="84" t="s">
@@ -5224,14 +5242,14 @@
       </c>
     </row>
     <row r="55" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A55" s="100" t="s">
+      <c r="A55" s="96" t="s">
         <v>344</v>
       </c>
-      <c r="B55" s="100" t="str">
+      <c r="B55" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0054</v>
       </c>
-      <c r="C55" s="113" t="s">
+      <c r="C55" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D55" s="85" t="s">
@@ -5240,7 +5258,7 @@
       <c r="E55" s="85" t="s">
         <v>83</v>
       </c>
-      <c r="F55" s="114" t="s">
+      <c r="F55" s="110" t="s">
         <v>242</v>
       </c>
       <c r="G55" s="85" t="s">
@@ -5257,14 +5275,14 @@
       </c>
     </row>
     <row r="56" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A56" s="100" t="s">
+      <c r="A56" s="96" t="s">
         <v>345</v>
       </c>
-      <c r="B56" s="100" t="str">
+      <c r="B56" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0055</v>
       </c>
-      <c r="C56" s="113" t="s">
+      <c r="C56" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D56" s="85" t="s">
@@ -5273,14 +5291,14 @@
       <c r="E56" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="F56" s="114" t="s">
+      <c r="F56" s="110" t="s">
         <v>255</v>
       </c>
       <c r="G56" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="H56" s="113" t="s">
-        <v>465</v>
+      <c r="H56" s="109" t="s">
+        <v>463</v>
       </c>
       <c r="I56" s="84" t="s">
         <v>31</v>
@@ -5293,14 +5311,14 @@
       </c>
     </row>
     <row r="57" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A57" s="100" t="s">
+      <c r="A57" s="96" t="s">
         <v>346</v>
       </c>
-      <c r="B57" s="100" t="str">
+      <c r="B57" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0056</v>
       </c>
-      <c r="C57" s="113" t="s">
+      <c r="C57" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D57" s="85" t="s">
@@ -5309,13 +5327,13 @@
       <c r="E57" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="F57" s="114" t="s">
+      <c r="F57" s="110" t="s">
         <v>256</v>
       </c>
       <c r="G57" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="H57" s="115">
+      <c r="H57" s="111">
         <v>19.14</v>
       </c>
       <c r="I57" s="84" t="s">
@@ -5326,14 +5344,14 @@
       </c>
     </row>
     <row r="58" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A58" s="100" t="s">
+      <c r="A58" s="96" t="s">
         <v>347</v>
       </c>
-      <c r="B58" s="100" t="str">
+      <c r="B58" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0057</v>
       </c>
-      <c r="C58" s="115" t="s">
+      <c r="C58" s="111" t="s">
         <v>266</v>
       </c>
       <c r="D58" s="85" t="s">
@@ -5342,13 +5360,13 @@
       <c r="E58" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="F58" s="114" t="s">
+      <c r="F58" s="110" t="s">
         <v>243</v>
       </c>
       <c r="G58" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="H58" s="100" t="s">
+      <c r="H58" s="96" t="s">
         <v>441</v>
       </c>
       <c r="I58" s="84" t="s">
@@ -5359,14 +5377,14 @@
       </c>
     </row>
     <row r="59" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A59" s="100" t="s">
+      <c r="A59" s="96" t="s">
         <v>348</v>
       </c>
-      <c r="B59" s="100" t="str">
+      <c r="B59" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0058</v>
       </c>
-      <c r="C59" s="113" t="s">
+      <c r="C59" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D59" s="85" t="s">
@@ -5375,13 +5393,13 @@
       <c r="E59" s="85" t="s">
         <v>87</v>
       </c>
-      <c r="F59" s="114" t="s">
+      <c r="F59" s="110" t="s">
         <v>244</v>
       </c>
       <c r="G59" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="H59" s="100" t="s">
+      <c r="H59" s="96" t="s">
         <v>442</v>
       </c>
       <c r="I59" s="84" t="s">
@@ -5392,23 +5410,23 @@
       </c>
     </row>
     <row r="60" spans="1:13" ht="64.5" hidden="1" thickBot="1">
-      <c r="A60" s="100" t="s">
+      <c r="A60" s="96" t="s">
         <v>349</v>
       </c>
-      <c r="B60" s="100" t="str">
+      <c r="B60" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0059</v>
       </c>
-      <c r="C60" s="113" t="s">
+      <c r="C60" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D60" s="85" t="s">
         <v>184</v>
       </c>
-      <c r="E60" s="112" t="s">
+      <c r="E60" s="108" t="s">
         <v>179</v>
       </c>
-      <c r="F60" s="114" t="s">
+      <c r="F60" s="110" t="s">
         <v>257</v>
       </c>
       <c r="G60" s="85"/>
@@ -5426,14 +5444,14 @@
       </c>
     </row>
     <row r="61" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A61" s="100" t="s">
+      <c r="A61" s="96" t="s">
         <v>350</v>
       </c>
-      <c r="B61" s="100" t="str">
+      <c r="B61" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0060</v>
       </c>
-      <c r="C61" s="113" t="s">
+      <c r="C61" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D61" s="85" t="s">
@@ -5442,13 +5460,13 @@
       <c r="E61" s="85" t="s">
         <v>180</v>
       </c>
-      <c r="F61" s="114" t="s">
+      <c r="F61" s="110" t="s">
         <v>258</v>
       </c>
       <c r="G61" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="H61" s="115">
+      <c r="H61" s="111">
         <v>10.1</v>
       </c>
       <c r="I61" s="84" t="s">
@@ -5460,14 +5478,14 @@
       </c>
     </row>
     <row r="62" spans="1:13" ht="39" thickBot="1">
-      <c r="A62" s="100" t="s">
+      <c r="A62" s="96" t="s">
         <v>351</v>
       </c>
-      <c r="B62" s="100" t="str">
+      <c r="B62" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0061</v>
       </c>
-      <c r="C62" s="113" t="s">
+      <c r="C62" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D62" s="85" t="s">
@@ -5476,13 +5494,13 @@
       <c r="E62" s="85" t="s">
         <v>88</v>
       </c>
-      <c r="F62" s="114" t="s">
+      <c r="F62" s="110" t="s">
         <v>259</v>
       </c>
       <c r="G62" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H62" s="102">
+      <c r="H62" s="98">
         <v>12.13</v>
       </c>
       <c r="I62" s="84" t="s">
@@ -5494,14 +5512,14 @@
       </c>
     </row>
     <row r="63" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A63" s="100" t="s">
+      <c r="A63" s="96" t="s">
         <v>352</v>
       </c>
-      <c r="B63" s="100" t="str">
+      <c r="B63" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0062</v>
       </c>
-      <c r="C63" s="113" t="s">
+      <c r="C63" s="109" t="s">
         <v>266</v>
       </c>
       <c r="D63" s="85" t="s">
@@ -5510,13 +5528,13 @@
       <c r="E63" s="85" t="s">
         <v>284</v>
       </c>
-      <c r="F63" s="114" t="s">
+      <c r="F63" s="110" t="s">
         <v>245</v>
       </c>
       <c r="G63" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="H63" s="102">
+      <c r="H63" s="98">
         <v>12.2</v>
       </c>
       <c r="I63" s="84" t="s">
@@ -5528,14 +5546,14 @@
       </c>
     </row>
     <row r="64" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A64" s="100" t="s">
+      <c r="A64" s="96" t="s">
         <v>353</v>
       </c>
-      <c r="B64" s="100" t="str">
+      <c r="B64" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0063</v>
       </c>
-      <c r="C64" s="113" t="s">
+      <c r="C64" s="109" t="s">
         <v>266</v>
       </c>
       <c r="D64" s="85" t="s">
@@ -5544,14 +5562,14 @@
       <c r="E64" s="85" t="s">
         <v>281</v>
       </c>
-      <c r="F64" s="114" t="s">
+      <c r="F64" s="110" t="s">
         <v>246</v>
       </c>
       <c r="G64" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="H64" s="102">
-        <v>12.2</v>
+      <c r="H64" s="96" t="s">
+        <v>468</v>
       </c>
       <c r="I64" s="84" t="s">
         <v>31</v>
@@ -5562,15 +5580,15 @@
       </c>
     </row>
     <row r="65" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A65" s="100" t="s">
+      <c r="A65" s="96" t="s">
         <v>354</v>
       </c>
-      <c r="B65" s="100" t="str">
+      <c r="B65" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0064</v>
       </c>
-      <c r="C65" s="113" t="s">
-        <v>264</v>
+      <c r="C65" s="127" t="s">
+        <v>266</v>
       </c>
       <c r="D65" s="85" t="s">
         <v>166</v>
@@ -5578,11 +5596,14 @@
       <c r="E65" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="F65" s="114" t="s">
+      <c r="F65" s="110" t="s">
         <v>260</v>
       </c>
       <c r="G65" s="85" t="s">
-        <v>405</v>
+        <v>263</v>
+      </c>
+      <c r="H65" s="109" t="s">
+        <v>469</v>
       </c>
       <c r="I65" s="84" t="s">
         <v>31</v>
@@ -5591,19 +5612,16 @@
       <c r="L65" s="88" t="s">
         <v>269</v>
       </c>
-      <c r="M65" s="86" t="s">
-        <v>443</v>
-      </c>
     </row>
     <row r="66" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A66" s="100" t="s">
+      <c r="A66" s="96" t="s">
         <v>355</v>
       </c>
-      <c r="B66" s="100" t="str">
+      <c r="B66" s="96" t="str">
         <f t="shared" si="0"/>
         <v>131_0065</v>
       </c>
-      <c r="C66" s="113" t="s">
+      <c r="C66" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D66" s="85" t="s">
@@ -5612,13 +5630,13 @@
       <c r="E66" s="85" t="s">
         <v>89</v>
       </c>
-      <c r="F66" s="114" t="s">
+      <c r="F66" s="110" t="s">
         <v>261</v>
       </c>
       <c r="G66" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H66" s="102">
+      <c r="H66" s="98">
         <v>12.13</v>
       </c>
       <c r="I66" s="84" t="s">
@@ -5630,14 +5648,14 @@
       </c>
     </row>
     <row r="67" spans="1:13" ht="26.25" hidden="1" thickBot="1">
-      <c r="A67" s="100" t="s">
+      <c r="A67" s="96" t="s">
         <v>356</v>
       </c>
-      <c r="B67" s="100" t="str">
-        <f t="shared" ref="B67:B102" si="1">_xlfn.CONCAT("131_", TEXT(ROW()-1, "0000"))</f>
+      <c r="B67" s="96" t="str">
+        <f t="shared" ref="B67:B101" si="1">_xlfn.CONCAT("131_", TEXT(ROW()-1, "0000"))</f>
         <v>131_0066</v>
       </c>
-      <c r="C67" s="113" t="s">
+      <c r="C67" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D67" s="85" t="s">
@@ -5646,7 +5664,7 @@
       <c r="E67" s="85" t="s">
         <v>90</v>
       </c>
-      <c r="F67" s="114" t="s">
+      <c r="F67" s="110" t="s">
         <v>262</v>
       </c>
       <c r="G67" s="85"/>
@@ -5664,14 +5682,14 @@
       </c>
     </row>
     <row r="68" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A68" s="100" t="s">
+      <c r="A68" s="96" t="s">
         <v>357</v>
       </c>
-      <c r="B68" s="100" t="str">
+      <c r="B68" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0067</v>
       </c>
-      <c r="C68" s="113" t="s">
+      <c r="C68" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D68" s="85" t="s">
@@ -5680,14 +5698,14 @@
       <c r="E68" s="85" t="s">
         <v>91</v>
       </c>
-      <c r="F68" s="114" t="s">
+      <c r="F68" s="110" t="s">
         <v>247</v>
       </c>
       <c r="G68" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="H68" s="100" t="s">
-        <v>444</v>
+      <c r="H68" s="96" t="s">
+        <v>443</v>
       </c>
       <c r="I68" s="84" t="s">
         <v>31</v>
@@ -5697,14 +5715,14 @@
       </c>
     </row>
     <row r="69" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A69" s="100" t="s">
+      <c r="A69" s="96" t="s">
         <v>358</v>
       </c>
-      <c r="B69" s="100" t="str">
+      <c r="B69" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0068</v>
       </c>
-      <c r="C69" s="113" t="s">
+      <c r="C69" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D69" s="85" t="s">
@@ -5713,14 +5731,14 @@
       <c r="E69" s="85" t="s">
         <v>92</v>
       </c>
-      <c r="F69" s="114" t="s">
+      <c r="F69" s="110" t="s">
         <v>248</v>
       </c>
       <c r="G69" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="H69" s="100" t="s">
-        <v>444</v>
+      <c r="H69" s="96" t="s">
+        <v>443</v>
       </c>
       <c r="I69" s="84" t="s">
         <v>31</v>
@@ -5730,14 +5748,14 @@
       </c>
     </row>
     <row r="70" spans="1:13" ht="39" thickBot="1">
-      <c r="A70" s="100" t="s">
+      <c r="A70" s="96" t="s">
         <v>359</v>
       </c>
-      <c r="B70" s="100" t="str">
+      <c r="B70" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0069</v>
       </c>
-      <c r="C70" s="113" t="s">
+      <c r="C70" s="109" t="s">
         <v>266</v>
       </c>
       <c r="D70" s="85" t="s">
@@ -5746,14 +5764,14 @@
       <c r="E70" s="85" t="s">
         <v>93</v>
       </c>
-      <c r="F70" s="114" t="s">
+      <c r="F70" s="110" t="s">
         <v>249</v>
       </c>
       <c r="G70" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="H70" s="100" t="s">
-        <v>444</v>
+      <c r="H70" s="96" t="s">
+        <v>443</v>
       </c>
       <c r="I70" s="84" t="s">
         <v>31</v>
@@ -5763,14 +5781,14 @@
       </c>
     </row>
     <row r="71" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A71" s="100" t="s">
+      <c r="A71" s="96" t="s">
         <v>360</v>
       </c>
-      <c r="B71" s="100" t="str">
+      <c r="B71" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0070</v>
       </c>
-      <c r="C71" s="113" t="s">
+      <c r="C71" s="109" t="s">
         <v>266</v>
       </c>
       <c r="D71" s="85" t="s">
@@ -5779,14 +5797,14 @@
       <c r="E71" s="85" t="s">
         <v>94</v>
       </c>
-      <c r="F71" s="114" t="s">
+      <c r="F71" s="110" t="s">
         <v>250</v>
       </c>
       <c r="G71" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="H71" s="100" t="s">
-        <v>445</v>
+      <c r="H71" s="96" t="s">
+        <v>444</v>
       </c>
       <c r="I71" s="84" t="s">
         <v>31</v>
@@ -5796,14 +5814,14 @@
       </c>
     </row>
     <row r="72" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A72" s="100" t="s">
+      <c r="A72" s="96" t="s">
         <v>361</v>
       </c>
-      <c r="B72" s="100" t="str">
+      <c r="B72" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0071</v>
       </c>
-      <c r="C72" s="113" t="s">
+      <c r="C72" s="109" t="s">
         <v>266</v>
       </c>
       <c r="D72" s="85" t="s">
@@ -5812,14 +5830,14 @@
       <c r="E72" s="85" t="s">
         <v>95</v>
       </c>
-      <c r="F72" s="114" t="s">
+      <c r="F72" s="110" t="s">
         <v>250</v>
       </c>
       <c r="G72" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="H72" s="100" t="s">
-        <v>445</v>
+      <c r="H72" s="96" t="s">
+        <v>444</v>
       </c>
       <c r="I72" s="84" t="s">
         <v>31</v>
@@ -5829,14 +5847,14 @@
       </c>
     </row>
     <row r="73" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A73" s="100" t="s">
+      <c r="A73" s="96" t="s">
         <v>362</v>
       </c>
-      <c r="B73" s="100" t="str">
+      <c r="B73" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0072</v>
       </c>
-      <c r="C73" s="113" t="s">
+      <c r="C73" s="109" t="s">
         <v>266</v>
       </c>
       <c r="D73" s="85" t="s">
@@ -5845,13 +5863,13 @@
       <c r="E73" s="85" t="s">
         <v>287</v>
       </c>
-      <c r="F73" s="114" t="s">
+      <c r="F73" s="110" t="s">
         <v>251</v>
       </c>
       <c r="G73" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="H73" s="102" t="s">
+      <c r="H73" s="98" t="s">
         <v>279</v>
       </c>
       <c r="I73" s="84" t="s">
@@ -5868,14 +5886,14 @@
       </c>
     </row>
     <row r="74" spans="1:13" ht="26.25" hidden="1" thickBot="1">
-      <c r="A74" s="100" t="s">
+      <c r="A74" s="96" t="s">
         <v>363</v>
       </c>
-      <c r="B74" s="100" t="str">
+      <c r="B74" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0073</v>
       </c>
-      <c r="C74" s="113" t="s">
+      <c r="C74" s="109" t="s">
         <v>265</v>
       </c>
       <c r="D74" s="85" t="s">
@@ -5884,7 +5902,7 @@
       <c r="E74" s="85" t="s">
         <v>96</v>
       </c>
-      <c r="F74" s="114" t="s">
+      <c r="F74" s="110" t="s">
         <v>252</v>
       </c>
       <c r="G74" s="85" t="s">
@@ -5904,14 +5922,14 @@
       </c>
     </row>
     <row r="75" spans="1:13" ht="39" hidden="1" thickBot="1">
-      <c r="A75" s="100" t="s">
+      <c r="A75" s="96" t="s">
         <v>364</v>
       </c>
-      <c r="B75" s="100" t="str">
+      <c r="B75" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0074</v>
       </c>
-      <c r="C75" s="113" t="s">
+      <c r="C75" s="109" t="s">
         <v>265</v>
       </c>
       <c r="D75" s="85" t="s">
@@ -5920,7 +5938,7 @@
       <c r="E75" s="85" t="s">
         <v>97</v>
       </c>
-      <c r="F75" s="114" t="s">
+      <c r="F75" s="110" t="s">
         <v>253</v>
       </c>
       <c r="G75" s="85" t="s">
@@ -5940,23 +5958,23 @@
       </c>
     </row>
     <row r="76" spans="1:13" ht="26.25" hidden="1" thickBot="1">
-      <c r="A76" s="100" t="s">
+      <c r="A76" s="96" t="s">
         <v>365</v>
       </c>
-      <c r="B76" s="100" t="str">
+      <c r="B76" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0075</v>
       </c>
-      <c r="C76" s="113" t="s">
+      <c r="C76" s="109" t="s">
         <v>265</v>
       </c>
-      <c r="D76" s="112" t="s">
+      <c r="D76" s="108" t="s">
         <v>175</v>
       </c>
       <c r="E76" s="85" t="s">
         <v>98</v>
       </c>
-      <c r="F76" s="114" t="s">
+      <c r="F76" s="110" t="s">
         <v>253</v>
       </c>
       <c r="G76" s="85" t="s">
@@ -5976,23 +5994,23 @@
       </c>
     </row>
     <row r="77" spans="1:13" ht="26.25" hidden="1" thickBot="1">
-      <c r="A77" s="100" t="s">
+      <c r="A77" s="96" t="s">
         <v>366</v>
       </c>
-      <c r="B77" s="100" t="str">
+      <c r="B77" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0076</v>
       </c>
-      <c r="C77" s="113" t="s">
+      <c r="C77" s="109" t="s">
         <v>265</v>
       </c>
-      <c r="D77" s="112" t="s">
+      <c r="D77" s="108" t="s">
         <v>175</v>
       </c>
       <c r="E77" s="85" t="s">
         <v>99</v>
       </c>
-      <c r="F77" s="114" t="s">
+      <c r="F77" s="110" t="s">
         <v>253</v>
       </c>
       <c r="G77" s="85" t="s">
@@ -6012,23 +6030,23 @@
       </c>
     </row>
     <row r="78" spans="1:13" ht="26.25" hidden="1" thickBot="1">
-      <c r="A78" s="100" t="s">
+      <c r="A78" s="96" t="s">
         <v>367</v>
       </c>
-      <c r="B78" s="100" t="str">
+      <c r="B78" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0077</v>
       </c>
-      <c r="C78" s="113" t="s">
+      <c r="C78" s="109" t="s">
         <v>265</v>
       </c>
-      <c r="D78" s="112" t="s">
+      <c r="D78" s="108" t="s">
         <v>176</v>
       </c>
       <c r="E78" s="85" t="s">
         <v>100</v>
       </c>
-      <c r="F78" s="114" t="s">
+      <c r="F78" s="110" t="s">
         <v>253</v>
       </c>
       <c r="G78" s="85" t="s">
@@ -6048,23 +6066,23 @@
       </c>
     </row>
     <row r="79" spans="1:13" ht="26.25" hidden="1" thickBot="1">
-      <c r="A79" s="100" t="s">
+      <c r="A79" s="96" t="s">
         <v>368</v>
       </c>
-      <c r="B79" s="100" t="str">
+      <c r="B79" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0078</v>
       </c>
-      <c r="C79" s="113" t="s">
+      <c r="C79" s="109" t="s">
         <v>265</v>
       </c>
-      <c r="D79" s="112" t="s">
+      <c r="D79" s="108" t="s">
         <v>177</v>
       </c>
       <c r="E79" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="F79" s="114" t="s">
+      <c r="F79" s="110" t="s">
         <v>253</v>
       </c>
       <c r="G79" s="85" t="s">
@@ -6084,23 +6102,23 @@
       </c>
     </row>
     <row r="80" spans="1:13" ht="26.25" hidden="1" thickBot="1">
-      <c r="A80" s="100" t="s">
+      <c r="A80" s="96" t="s">
         <v>369</v>
       </c>
-      <c r="B80" s="100" t="str">
+      <c r="B80" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0079</v>
       </c>
-      <c r="C80" s="113" t="s">
+      <c r="C80" s="109" t="s">
         <v>265</v>
       </c>
-      <c r="D80" s="112" t="s">
+      <c r="D80" s="108" t="s">
         <v>175</v>
       </c>
       <c r="E80" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="F80" s="114" t="s">
+      <c r="F80" s="110" t="s">
         <v>253</v>
       </c>
       <c r="G80" s="85" t="s">
@@ -6120,23 +6138,23 @@
       </c>
     </row>
     <row r="81" spans="1:13" ht="26.25" hidden="1" thickBot="1">
-      <c r="A81" s="100" t="s">
+      <c r="A81" s="96" t="s">
         <v>370</v>
       </c>
-      <c r="B81" s="100" t="str">
+      <c r="B81" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0080</v>
       </c>
-      <c r="C81" s="113" t="s">
+      <c r="C81" s="109" t="s">
         <v>265</v>
       </c>
-      <c r="D81" s="112" t="s">
+      <c r="D81" s="108" t="s">
         <v>187</v>
       </c>
       <c r="E81" s="85" t="s">
         <v>103</v>
       </c>
-      <c r="F81" s="114" t="s">
+      <c r="F81" s="110" t="s">
         <v>253</v>
       </c>
       <c r="G81" s="85" t="s">
@@ -6156,23 +6174,23 @@
       </c>
     </row>
     <row r="82" spans="1:13" ht="26.25" hidden="1" thickBot="1">
-      <c r="A82" s="100" t="s">
+      <c r="A82" s="96" t="s">
         <v>371</v>
       </c>
-      <c r="B82" s="100" t="str">
+      <c r="B82" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0081</v>
       </c>
-      <c r="C82" s="113" t="s">
+      <c r="C82" s="109" t="s">
         <v>265</v>
       </c>
-      <c r="D82" s="112" t="s">
+      <c r="D82" s="108" t="s">
         <v>188</v>
       </c>
       <c r="E82" s="85" t="s">
         <v>104</v>
       </c>
-      <c r="F82" s="114" t="s">
+      <c r="F82" s="110" t="s">
         <v>253</v>
       </c>
       <c r="G82" s="85" t="s">
@@ -6192,23 +6210,23 @@
       </c>
     </row>
     <row r="83" spans="1:13" ht="39" hidden="1" thickBot="1">
-      <c r="A83" s="100" t="s">
+      <c r="A83" s="96" t="s">
         <v>372</v>
       </c>
-      <c r="B83" s="100" t="str">
+      <c r="B83" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0082</v>
       </c>
-      <c r="C83" s="113" t="s">
+      <c r="C83" s="109" t="s">
         <v>265</v>
       </c>
-      <c r="D83" s="112" t="s">
+      <c r="D83" s="108" t="s">
         <v>189</v>
       </c>
       <c r="E83" s="85" t="s">
         <v>105</v>
       </c>
-      <c r="F83" s="114" t="s">
+      <c r="F83" s="110" t="s">
         <v>253</v>
       </c>
       <c r="G83" s="85" t="s">
@@ -6228,23 +6246,23 @@
       </c>
     </row>
     <row r="84" spans="1:13" ht="39" hidden="1" thickBot="1">
-      <c r="A84" s="100" t="s">
+      <c r="A84" s="96" t="s">
         <v>373</v>
       </c>
-      <c r="B84" s="100" t="str">
+      <c r="B84" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0083</v>
       </c>
-      <c r="C84" s="113" t="s">
+      <c r="C84" s="109" t="s">
         <v>265</v>
       </c>
-      <c r="D84" s="112" t="s">
+      <c r="D84" s="108" t="s">
         <v>190</v>
       </c>
       <c r="E84" s="85" t="s">
         <v>106</v>
       </c>
-      <c r="F84" s="114" t="s">
+      <c r="F84" s="110" t="s">
         <v>253</v>
       </c>
       <c r="G84" s="85" t="s">
@@ -6264,23 +6282,23 @@
       </c>
     </row>
     <row r="85" spans="1:13" ht="26.25" hidden="1" thickBot="1">
-      <c r="A85" s="100" t="s">
+      <c r="A85" s="96" t="s">
         <v>374</v>
       </c>
-      <c r="B85" s="100" t="str">
+      <c r="B85" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0084</v>
       </c>
-      <c r="C85" s="113" t="s">
+      <c r="C85" s="109" t="s">
         <v>265</v>
       </c>
-      <c r="D85" s="112" t="s">
+      <c r="D85" s="108" t="s">
         <v>191</v>
       </c>
       <c r="E85" s="85" t="s">
         <v>107</v>
       </c>
-      <c r="F85" s="114" t="s">
+      <c r="F85" s="110" t="s">
         <v>253</v>
       </c>
       <c r="G85" s="85" t="s">
@@ -6300,30 +6318,30 @@
       </c>
     </row>
     <row r="86" spans="1:13" ht="39" thickBot="1">
-      <c r="A86" s="100" t="s">
+      <c r="A86" s="96" t="s">
         <v>375</v>
       </c>
-      <c r="B86" s="100" t="str">
+      <c r="B86" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0085</v>
       </c>
-      <c r="C86" s="113" t="s">
+      <c r="C86" s="109" t="s">
         <v>266</v>
       </c>
-      <c r="D86" s="112" t="s">
+      <c r="D86" s="108" t="s">
         <v>178</v>
       </c>
       <c r="E86" s="85" t="s">
         <v>108</v>
       </c>
-      <c r="F86" s="120" t="s">
-        <v>446</v>
+      <c r="F86" s="116" t="s">
+        <v>445</v>
       </c>
       <c r="G86" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="H86" s="100" t="s">
-        <v>464</v>
+      <c r="H86" s="96" t="s">
+        <v>462</v>
       </c>
       <c r="I86" s="84" t="s">
         <v>31</v>
@@ -6332,34 +6350,34 @@
         <v>267</v>
       </c>
       <c r="M86" s="86" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A87" s="100" t="str">
+      <c r="A87" s="96" t="str">
         <f>_xlfn.CONCAT("131_ED2_", TEXT(ROW()-86,"000"))</f>
         <v>131_ED2_001</v>
       </c>
-      <c r="B87" s="100" t="str">
+      <c r="B87" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0086</v>
       </c>
-      <c r="C87" s="113" t="s">
+      <c r="C87" s="109" t="s">
         <v>266</v>
       </c>
-      <c r="D87" s="117" t="s">
+      <c r="D87" s="113" t="s">
         <v>391</v>
       </c>
-      <c r="E87" s="117" t="s">
+      <c r="E87" s="113" t="s">
         <v>392</v>
       </c>
-      <c r="F87" s="114" t="s">
+      <c r="F87" s="110" t="s">
         <v>393</v>
       </c>
-      <c r="G87" s="117" t="s">
+      <c r="G87" s="113" t="s">
         <v>25</v>
       </c>
-      <c r="H87" s="115">
+      <c r="H87" s="111">
         <v>7.6</v>
       </c>
       <c r="I87" s="84" t="s">
@@ -6372,30 +6390,30 @@
       <c r="M87" s="87"/>
     </row>
     <row r="88" spans="1:13" ht="39" thickBot="1">
-      <c r="A88" s="100" t="str">
-        <f t="shared" ref="A88:A102" si="2">_xlfn.CONCAT("131_ED2_", TEXT(ROW()-86,"000"))</f>
+      <c r="A88" s="96" t="str">
+        <f t="shared" ref="A88:A101" si="2">_xlfn.CONCAT("131_ED2_", TEXT(ROW()-86,"000"))</f>
         <v>131_ED2_002</v>
       </c>
-      <c r="B88" s="100" t="str">
+      <c r="B88" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0087</v>
       </c>
-      <c r="C88" s="113" t="s">
+      <c r="C88" s="109" t="s">
         <v>265</v>
       </c>
-      <c r="D88" s="110" t="s">
+      <c r="D88" s="106" t="s">
         <v>395</v>
       </c>
       <c r="E88" s="85" t="s">
         <v>396</v>
       </c>
-      <c r="F88" s="114" t="s">
+      <c r="F88" s="110" t="s">
         <v>397</v>
       </c>
       <c r="G88" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H88" s="102">
+      <c r="H88" s="98">
         <v>7.5</v>
       </c>
       <c r="I88" s="84" t="s">
@@ -6410,15 +6428,15 @@
       </c>
     </row>
     <row r="89" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A89" s="100" t="str">
+      <c r="A89" s="96" t="str">
         <f t="shared" si="2"/>
         <v>131_ED2_003</v>
       </c>
-      <c r="B89" s="100" t="str">
+      <c r="B89" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0088</v>
       </c>
-      <c r="C89" s="113" t="s">
+      <c r="C89" s="109" t="s">
         <v>266</v>
       </c>
       <c r="D89" s="85" t="s">
@@ -6427,13 +6445,13 @@
       <c r="E89" s="85" t="s">
         <v>399</v>
       </c>
-      <c r="F89" s="114" t="s">
+      <c r="F89" s="110" t="s">
         <v>400</v>
       </c>
       <c r="G89" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H89" s="102">
+      <c r="H89" s="98">
         <v>7.3</v>
       </c>
       <c r="I89" s="84" t="s">
@@ -6444,290 +6462,287 @@
         <v>268</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="39" thickBot="1">
-      <c r="A90" s="100" t="str">
+    <row r="90" spans="1:13" ht="26.25" thickBot="1">
+      <c r="A90" s="96" t="str">
         <f t="shared" si="2"/>
         <v>131_ED2_004</v>
       </c>
-      <c r="B90" s="100" t="str">
+      <c r="B90" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0089</v>
       </c>
-      <c r="C90" s="113" t="s">
+      <c r="C90" s="100" t="s">
         <v>264</v>
       </c>
       <c r="D90" s="85" t="s">
-        <v>111</v>
+        <v>402</v>
       </c>
       <c r="E90" s="85" t="s">
-        <v>40</v>
-      </c>
-      <c r="F90" s="101" t="s">
-        <v>194</v>
+        <v>403</v>
+      </c>
+      <c r="F90" s="114" t="s">
+        <v>401</v>
       </c>
       <c r="G90" s="85" t="s">
-        <v>263</v>
-      </c>
-      <c r="H90" s="100" t="s">
-        <v>448</v>
-      </c>
-      <c r="I90" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="H90" s="96">
+        <v>12.8</v>
+      </c>
+      <c r="I90" s="91" t="s">
         <v>26</v>
       </c>
+      <c r="J90" s="92"/>
+      <c r="K90" s="92"/>
       <c r="L90" s="85" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="91" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A91" s="100" t="str">
+      <c r="A91" s="96" t="str">
         <f t="shared" si="2"/>
         <v>131_ED2_005</v>
       </c>
-      <c r="B91" s="100" t="str">
+      <c r="B91" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0090</v>
       </c>
-      <c r="C91" s="104" t="s">
-        <v>264</v>
+      <c r="C91" s="96" t="s">
+        <v>265</v>
       </c>
       <c r="D91" s="85" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="E91" s="85" t="s">
-        <v>403</v>
-      </c>
-      <c r="F91" s="118" t="s">
-        <v>401</v>
+        <v>410</v>
+      </c>
+      <c r="F91" s="116" t="s">
+        <v>411</v>
       </c>
       <c r="G91" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H91" s="128">
-        <v>12.8</v>
-      </c>
-      <c r="I91" s="91" t="s">
+      <c r="H91" s="96">
+        <v>13.1</v>
+      </c>
+      <c r="I91" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="J91" s="92"/>
-      <c r="K91" s="92"/>
-      <c r="L91" s="85" t="s">
-        <v>270</v>
-      </c>
     </row>
     <row r="92" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A92" s="100" t="str">
+      <c r="A92" s="96" t="str">
         <f t="shared" si="2"/>
         <v>131_ED2_006</v>
       </c>
-      <c r="B92" s="100" t="str">
+      <c r="B92" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0091</v>
       </c>
-      <c r="C92" s="100" t="s">
+      <c r="C92" s="96" t="s">
         <v>265</v>
       </c>
       <c r="D92" s="85" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="E92" s="85" t="s">
-        <v>410</v>
-      </c>
-      <c r="F92" s="120" t="s">
-        <v>411</v>
+        <v>413</v>
+      </c>
+      <c r="F92" s="116" t="s">
+        <v>414</v>
       </c>
       <c r="G92" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H92" s="100">
+      <c r="H92" s="96">
         <v>13.1</v>
       </c>
       <c r="I92" s="92" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A93" s="100" t="str">
+    <row r="93" spans="1:13" ht="39" thickBot="1">
+      <c r="A93" s="96" t="str">
         <f t="shared" si="2"/>
         <v>131_ED2_007</v>
       </c>
-      <c r="B93" s="100" t="str">
+      <c r="B93" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0092</v>
       </c>
-      <c r="C93" s="100" t="s">
+      <c r="C93" s="96" t="s">
         <v>265</v>
       </c>
-      <c r="D93" s="85" t="s">
-        <v>412</v>
-      </c>
-      <c r="E93" s="85" t="s">
-        <v>413</v>
-      </c>
-      <c r="F93" s="120" t="s">
-        <v>414</v>
+      <c r="D93" s="115" t="s">
+        <v>415</v>
+      </c>
+      <c r="E93" s="115" t="s">
+        <v>416</v>
+      </c>
+      <c r="F93" s="117" t="s">
+        <v>417</v>
       </c>
       <c r="G93" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="H93" s="100">
+      <c r="H93" s="96">
         <v>13.1</v>
       </c>
       <c r="I93" s="92" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="39" thickBot="1">
-      <c r="A94" s="100" t="str">
+    <row r="94" spans="1:13" ht="26.25" thickBot="1">
+      <c r="A94" s="96" t="str">
         <f t="shared" si="2"/>
         <v>131_ED2_008</v>
       </c>
-      <c r="B94" s="100" t="str">
+      <c r="B94" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0093</v>
       </c>
-      <c r="C94" s="100" t="s">
+      <c r="C94" s="96" t="s">
         <v>265</v>
       </c>
-      <c r="D94" s="119" t="s">
-        <v>415</v>
-      </c>
-      <c r="E94" s="119" t="s">
-        <v>416</v>
-      </c>
-      <c r="F94" s="121" t="s">
-        <v>417</v>
-      </c>
-      <c r="G94" s="85" t="s">
+      <c r="D94" s="116" t="s">
+        <v>418</v>
+      </c>
+      <c r="E94" s="116" t="s">
+        <v>419</v>
+      </c>
+      <c r="F94" s="116" t="s">
+        <v>239</v>
+      </c>
+      <c r="G94" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="H94" s="100">
-        <v>13.1</v>
+      <c r="H94" s="96">
+        <v>14.1</v>
       </c>
       <c r="I94" s="92" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A95" s="100" t="str">
+    <row r="95" spans="1:13" ht="39" thickBot="1">
+      <c r="A95" s="96" t="str">
         <f t="shared" si="2"/>
         <v>131_ED2_009</v>
       </c>
-      <c r="B95" s="100" t="str">
+      <c r="B95" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0094</v>
       </c>
-      <c r="C95" s="100" t="s">
-        <v>265</v>
-      </c>
-      <c r="D95" s="120" t="s">
-        <v>418</v>
-      </c>
-      <c r="E95" s="120" t="s">
-        <v>419</v>
-      </c>
-      <c r="F95" s="120" t="s">
-        <v>239</v>
-      </c>
-      <c r="G95" s="122" t="s">
+      <c r="C95" s="109" t="s">
+        <v>266</v>
+      </c>
+      <c r="D95" s="91" t="s">
+        <v>423</v>
+      </c>
+      <c r="E95" s="91" t="s">
+        <v>422</v>
+      </c>
+      <c r="F95" s="91" t="s">
+        <v>424</v>
+      </c>
+      <c r="G95" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="H95" s="100">
-        <v>14.1</v>
+      <c r="H95" s="109" t="s">
+        <v>278</v>
       </c>
       <c r="I95" s="92" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="96" spans="1:13" ht="39" thickBot="1">
-      <c r="A96" s="100" t="str">
+      <c r="L95" s="91" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" ht="26.25" thickBot="1">
+      <c r="A96" s="96" t="str">
         <f t="shared" si="2"/>
         <v>131_ED2_010</v>
       </c>
-      <c r="B96" s="100" t="str">
+      <c r="B96" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0095</v>
       </c>
-      <c r="C96" s="113" t="s">
-        <v>266</v>
+      <c r="C96" s="109" t="s">
+        <v>264</v>
       </c>
       <c r="D96" s="91" t="s">
-        <v>423</v>
+        <v>448</v>
       </c>
       <c r="E96" s="91" t="s">
-        <v>422</v>
+        <v>447</v>
       </c>
       <c r="F96" s="91" t="s">
-        <v>424</v>
-      </c>
-      <c r="G96" s="123" t="s">
+        <v>449</v>
+      </c>
+      <c r="G96" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="H96" s="113" t="s">
-        <v>278</v>
+      <c r="H96" s="111">
+        <v>7.3</v>
       </c>
       <c r="I96" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="L96" s="91" t="s">
-        <v>269</v>
-      </c>
     </row>
     <row r="97" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A97" s="100" t="str">
+      <c r="A97" s="96" t="str">
         <f t="shared" si="2"/>
         <v>131_ED2_011</v>
       </c>
-      <c r="B97" s="100" t="str">
+      <c r="B97" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0096</v>
       </c>
-      <c r="C97" s="113" t="s">
+      <c r="C97" s="109" t="s">
         <v>264</v>
       </c>
       <c r="D97" s="91" t="s">
+        <v>451</v>
+      </c>
+      <c r="E97" s="91" t="s">
         <v>450</v>
       </c>
-      <c r="E97" s="91" t="s">
-        <v>449</v>
-      </c>
       <c r="F97" s="91" t="s">
-        <v>451</v>
-      </c>
-      <c r="G97" s="123" t="s">
-        <v>25</v>
-      </c>
-      <c r="H97" s="115">
-        <v>7.3</v>
+        <v>452</v>
+      </c>
+      <c r="G97" s="119" t="s">
+        <v>263</v>
+      </c>
+      <c r="H97" s="109" t="s">
+        <v>275</v>
       </c>
       <c r="I97" s="92" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="98" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A98" s="100" t="str">
+      <c r="A98" s="96" t="str">
         <f t="shared" si="2"/>
         <v>131_ED2_012</v>
       </c>
-      <c r="B98" s="100" t="str">
+      <c r="B98" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0097</v>
       </c>
-      <c r="C98" s="113" t="s">
-        <v>264</v>
+      <c r="C98" s="109" t="s">
+        <v>266</v>
       </c>
       <c r="D98" s="91" t="s">
         <v>453</v>
       </c>
       <c r="E98" s="91" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="F98" s="91" t="s">
-        <v>454</v>
-      </c>
-      <c r="G98" s="123" t="s">
+        <v>456</v>
+      </c>
+      <c r="G98" s="119" t="s">
         <v>263</v>
       </c>
-      <c r="H98" s="113" t="s">
+      <c r="H98" s="109" t="s">
         <v>275</v>
       </c>
       <c r="I98" s="92" t="s">
@@ -6735,137 +6750,107 @@
       </c>
     </row>
     <row r="99" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A99" s="100" t="str">
+      <c r="A99" s="96" t="str">
         <f t="shared" si="2"/>
         <v>131_ED2_013</v>
       </c>
-      <c r="B99" s="100" t="str">
+      <c r="B99" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0098</v>
       </c>
-      <c r="C99" s="113" t="s">
-        <v>266</v>
+      <c r="C99" s="109" t="s">
+        <v>264</v>
       </c>
       <c r="D99" s="91" t="s">
+        <v>460</v>
+      </c>
+      <c r="E99" s="91" t="s">
         <v>455</v>
       </c>
-      <c r="E99" s="91" t="s">
-        <v>456</v>
-      </c>
       <c r="F99" s="91" t="s">
-        <v>458</v>
-      </c>
-      <c r="G99" s="123" t="s">
+        <v>457</v>
+      </c>
+      <c r="G99" s="119" t="s">
         <v>263</v>
       </c>
-      <c r="H99" s="113" t="s">
-        <v>275</v>
+      <c r="H99" s="109" t="s">
+        <v>463</v>
       </c>
       <c r="I99" s="92" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="100" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A100" s="100" t="str">
+      <c r="A100" s="96" t="str">
         <f t="shared" si="2"/>
         <v>131_ED2_014</v>
       </c>
-      <c r="B100" s="100" t="str">
+      <c r="B100" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0099</v>
       </c>
-      <c r="C100" s="113" t="s">
-        <v>264</v>
+      <c r="C100" s="109" t="s">
+        <v>266</v>
       </c>
       <c r="D100" s="91" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E100" s="91" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="F100" s="91" t="s">
         <v>459</v>
       </c>
-      <c r="G100" s="123" t="s">
+      <c r="G100" s="119" t="s">
         <v>263</v>
       </c>
-      <c r="H100" s="113" t="s">
-        <v>465</v>
+      <c r="H100" s="109" t="s">
+        <v>463</v>
       </c>
       <c r="I100" s="92" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="101" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A101" s="100" t="str">
+      <c r="A101" s="96" t="str">
         <f t="shared" si="2"/>
         <v>131_ED2_015</v>
       </c>
-      <c r="B101" s="100" t="str">
+      <c r="B101" s="96" t="str">
         <f t="shared" si="1"/>
         <v>131_0100</v>
       </c>
-      <c r="C101" s="113" t="s">
+      <c r="C101" s="109" t="s">
         <v>266</v>
       </c>
       <c r="D101" s="91" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="E101" s="91" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="F101" s="91" t="s">
-        <v>461</v>
-      </c>
-      <c r="G101" s="123" t="s">
-        <v>263</v>
-      </c>
-      <c r="H101" s="113" t="s">
-        <v>465</v>
+        <v>466</v>
+      </c>
+      <c r="G101" s="119" t="s">
+        <v>405</v>
       </c>
       <c r="I101" s="92" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="102" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A102" s="100" t="str">
-        <f t="shared" si="2"/>
-        <v>131_ED2_016</v>
-      </c>
-      <c r="B102" s="100" t="str">
-        <f t="shared" si="1"/>
-        <v>131_0101</v>
-      </c>
-      <c r="C102" s="113" t="s">
-        <v>266</v>
-      </c>
-      <c r="D102" s="91" t="s">
-        <v>467</v>
-      </c>
-      <c r="E102" s="91" t="s">
-        <v>466</v>
-      </c>
-      <c r="F102" s="91" t="s">
-        <v>468</v>
-      </c>
-      <c r="G102" s="123" t="s">
-        <v>405</v>
-      </c>
-      <c r="I102" s="92" t="s">
-        <v>26</v>
-      </c>
-      <c r="M102" s="86" t="s">
+      <c r="M101" s="86" t="s">
         <v>432</v>
       </c>
     </row>
+    <row r="102" spans="1:13" ht="12.75"/>
   </sheetData>
-  <autoFilter ref="K1:K96" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <autoFilter ref="K1:K95" xr:uid="{00000000-0001-0000-0100-000000000000}">
     <filterColumn colId="0">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C32 C39:C269" xr:uid="{1FB138CC-14EF-4406-9E7B-EC5039F9ECE1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C32 C39:C268" xr:uid="{1FB138CC-14EF-4406-9E7B-EC5039F9ECE1}">
       <formula1>"C,E,W"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7074,7 +7059,7 @@
       </c>
       <c r="N4" s="43"/>
     </row>
-    <row r="5" spans="1:18" ht="26.25" thickBot="1">
+    <row r="5" spans="1:18" ht="39" thickBot="1">
       <c r="A5" s="44" t="str">
         <v>131_ED1_111</v>
       </c>
@@ -7116,7 +7101,7 @@
       </c>
       <c r="N5" s="43"/>
     </row>
-    <row r="6" spans="1:18" ht="13.5" thickBot="1">
+    <row r="6" spans="1:18" ht="26.25" thickBot="1">
       <c r="A6" s="44" t="str">
         <v>131_ED1_112</v>
       </c>
@@ -7158,7 +7143,7 @@
       </c>
       <c r="N6" s="43"/>
     </row>
-    <row r="7" spans="1:18" s="46" customFormat="1" ht="26.25" thickBot="1">
+    <row r="7" spans="1:18" s="46" customFormat="1" ht="13.5" thickBot="1">
       <c r="A7" s="44" t="str">
         <v>131_ED1_113</v>
       </c>
@@ -7324,7 +7309,7 @@
         <v>Covered by generic check(s) in S-158:100.</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="39" thickBot="1">
+    <row r="11" spans="1:18" ht="26.25" thickBot="1">
       <c r="A11" s="44" t="str">
         <v>131_ED1_117</v>
       </c>
@@ -7366,7 +7351,7 @@
       </c>
       <c r="N11" s="43"/>
     </row>
-    <row r="12" spans="1:18" ht="26.25" thickBot="1">
+    <row r="12" spans="1:18" ht="39" thickBot="1">
       <c r="A12" s="44" t="str">
         <v>131_ED1_118</v>
       </c>
@@ -7408,7 +7393,7 @@
       </c>
       <c r="N12" s="43"/>
     </row>
-    <row r="13" spans="1:18" s="46" customFormat="1" ht="39" thickBot="1">
+    <row r="13" spans="1:18" s="46" customFormat="1" ht="26.25" thickBot="1">
       <c r="A13" s="44" t="str">
         <v>131_ED1_128</v>
       </c>
@@ -7450,7 +7435,7 @@
       </c>
       <c r="N13" s="43"/>
     </row>
-    <row r="14" spans="1:18" s="46" customFormat="1" ht="26.25" thickBot="1">
+    <row r="14" spans="1:18" s="46" customFormat="1" ht="39" thickBot="1">
       <c r="A14" s="44" t="str">
         <v>131_ED1_129</v>
       </c>
@@ -7576,7 +7561,7 @@
       </c>
       <c r="N16" s="43"/>
     </row>
-    <row r="17" spans="1:14" ht="39" thickBot="1">
+    <row r="17" spans="1:14" ht="26.25" thickBot="1">
       <c r="A17" s="44" t="str">
         <v>131_ED1_133</v>
       </c>
@@ -7618,7 +7603,7 @@
       </c>
       <c r="N17" s="43"/>
     </row>
-    <row r="18" spans="1:14" ht="26.25" thickBot="1">
+    <row r="18" spans="1:14" ht="39" thickBot="1">
       <c r="A18" s="44" t="str">
         <v>131_ED1_134</v>
       </c>
@@ -7912,7 +7897,7 @@
       </c>
       <c r="N24" s="43"/>
     </row>
-    <row r="25" spans="1:14" ht="64.5" thickBot="1">
+    <row r="25" spans="1:14" ht="26.25" thickBot="1">
       <c r="A25" s="44" t="str">
         <v>131_ED1_150</v>
       </c>
@@ -7954,7 +7939,7 @@
       </c>
       <c r="N25" s="43"/>
     </row>
-    <row r="26" spans="1:14" ht="26.25" thickBot="1">
+    <row r="26" spans="1:14" ht="64.5" thickBot="1">
       <c r="A26" s="44" t="str">
         <v>131_ED1_159</v>
       </c>
@@ -8038,7 +8023,7 @@
       </c>
       <c r="N27" s="43"/>
     </row>
-    <row r="28" spans="1:14" ht="39" thickBot="1">
+    <row r="28" spans="1:14" ht="26.25" thickBot="1">
       <c r="A28" s="44" t="str">
         <v>131_ED1_173</v>
       </c>
@@ -8080,7 +8065,7 @@
       </c>
       <c r="N28" s="43"/>
     </row>
-    <row r="29" spans="1:14" ht="26.25" thickBot="1">
+    <row r="29" spans="1:14" ht="39" thickBot="1">
       <c r="A29" s="44" t="str">
         <v>131_ED1_174</v>
       </c>
@@ -8330,7 +8315,7 @@
         <v>Covered by generic check(s) in S-158:100.</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="39" thickBot="1">
+    <row r="35" spans="1:13" ht="26.25" thickBot="1">
       <c r="A35" s="44" t="str">
         <v>131_ED1_180</v>
       </c>
@@ -8371,7 +8356,7 @@
         <v>Covered by generic check(s) in S-158:100.</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="51.75" thickBot="1">
+    <row r="36" spans="1:13" ht="39" thickBot="1">
       <c r="A36" s="44" t="str">
         <v>131_ED1_181</v>
       </c>
@@ -8412,7 +8397,7 @@
         <v>Covered by generic check(s) in S-158:100.</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="39" thickBot="1">
+    <row r="37" spans="1:13" ht="51.75" thickBot="1">
       <c r="A37" s="44" t="str">
         <v>131_ED1_182</v>
       </c>
@@ -8453,7 +8438,7 @@
         <v>Covered by generic check(s) in S-158:100.</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="26.25" thickBot="1">
+    <row r="38" spans="1:13" ht="39" thickBot="1">
       <c r="A38" s="44" t="str">
         <v>131_ED1_183</v>
       </c>
@@ -8494,7 +8479,7 @@
         <v>Covered by generic check(s) in S-158:100.</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="13.5" thickBot="1">
+    <row r="39" spans="1:13" ht="26.25" thickBot="1">
       <c r="A39" s="44" t="str">
         <v>131_ED1_184</v>
       </c>

</xml_diff>